<commit_message>
add: transferring columns to a file
</commit_message>
<xml_diff>
--- a/unzipping_table.xlsx
+++ b/unzipping_table.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="labels_before_table" sheetId="1" state="visible" r:id="rId3"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="275">
   <si>
     <t xml:space="preserve">seller</t>
   </si>
@@ -95,6 +95,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">发货人</t>
     </r>
@@ -123,6 +124,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">（发货人）</t>
     </r>
@@ -148,6 +150,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">目的站</t>
     </r>
@@ -170,6 +173,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">卖家</t>
     </r>
@@ -189,6 +193,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">买主</t>
     </r>
@@ -214,6 +219,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">卖方</t>
     </r>
@@ -233,6 +239,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">买方</t>
     </r>
@@ -312,6 +319,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">目的车站</t>
     </r>
@@ -331,6 +339,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">发货人</t>
     </r>
@@ -359,6 +368,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">卖家</t>
     </r>
@@ -378,6 +388,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">买家</t>
     </r>
@@ -406,6 +417,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">运单发货人</t>
     </r>
@@ -425,6 +437,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">卖方</t>
     </r>
@@ -444,6 +457,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">买方</t>
     </r>
@@ -612,6 +626,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">商品原产国</t>
     </r>
@@ -669,6 +684,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">编号</t>
     </r>
@@ -741,6 +757,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">货物名称</t>
     </r>
@@ -845,6 +862,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">位数</t>
     </r>
@@ -951,6 +969,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">位数）</t>
     </r>
@@ -970,6 +989,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">商品原产地</t>
     </r>
@@ -992,6 +1012,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">单件数量</t>
     </r>
@@ -1080,6 +1101,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">货源国</t>
     </r>
@@ -1102,6 +1124,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">单件数</t>
     </r>
@@ -1136,6 +1159,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">（国外对应的</t>
     </r>
@@ -1153,6 +1177,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">）</t>
     </r>
@@ -1172,6 +1197,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">货源国</t>
     </r>
@@ -1189,6 +1215,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">英文</t>
     </r>
@@ -1206,6 +1233,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">俄文</t>
     </r>
@@ -1255,6 +1283,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">海关编码</t>
     </r>
@@ -1269,6 +1298,26 @@
     </r>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GOODSORIGIN/СТРАНАПРОИСХОЖДЕНИЯТОВАРА</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">（货源地）</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">НАИМЕНОВАНИЕТОВАРА</t>
   </si>
   <si>
@@ -1338,6 +1387,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">海关编码</t>
     </r>
@@ -1419,6 +1469,46 @@
     <t xml:space="preserve">КОЛ-ВО,МЕСТ</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">NETWEIGHTKG/ВЕСНЕТТОКГ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">（净重）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GROSSWEIGHTKG/ВЕСБРУТТОКГ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">（毛重）</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">UNITPRICE/ЦЕНАЗАЕД,USD</t>
   </si>
   <si>
@@ -1495,6 +1585,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">货物名称</t>
     </r>
@@ -1563,6 +1654,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">货物名，描述</t>
     </r>
@@ -1611,6 +1703,26 @@
     </r>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">AMOUNT/ОБЩАЯСТОИМОСТЬ,CNY</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">（总额）</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">КОДТНВЭДТС</t>
   </si>
   <si>
@@ -1628,6 +1740,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">货物名，描述</t>
     </r>
@@ -1645,6 +1758,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">英文</t>
     </r>
@@ -1662,6 +1776,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">俄文</t>
     </r>
@@ -1679,6 +1794,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">织物、薄膜、卷装货物、玻璃等货物必须标注</t>
     </r>
@@ -1693,6 +1809,66 @@
     </r>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">QTYPCS/КОЛ-ВОШТ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">（小件数）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">QTYOFPLACE/PALLET/КОЛ-ВОМЕСТ,ПАЛЛЕТ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">（大件数）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">PRICEPERPCS/ЦЕНАЗАШТ,CNY</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">（单价）</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">КОДТНВЭДТСЕАЭС</t>
   </si>
   <si>
@@ -1710,6 +1886,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">（中英俄品名）</t>
     </r>
@@ -1718,7 +1895,99 @@
     <t xml:space="preserve">КОДТОВАРАВСООТВЕТСТВИИСТНВЭД</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">DESCRIPTIONOFGOODS/ОПИСАНИЕТОВАРОВ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">（品名中</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">英</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">俄文）</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">（清关HS编码）HSCODE/КОДТНВЭДТС</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">HSCODE/КОДТНВЭДТС</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">俄罗斯的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">HSCODE10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">位</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">station</t>
@@ -1860,12 +2129,12 @@
       <sz val="14"/>
       <name val="Noto Sans CJK SC"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="14"/>
       <name val="Noto Sans CJK SC"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1917,7 +2186,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1934,11 +2203,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2075,7 +2348,7 @@
   </sheetPr>
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -2373,25 +2646,26 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K22"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K13" activeCellId="0" sqref="K13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="19.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="23.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="4" width="32.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="4" width="34.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="4" width="28.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="4" width="23.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="4" width="32.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="4" width="20.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="4" width="21.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="4" width="19.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="4" width="22.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="23.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="32.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="34.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="28.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="23.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="32.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="20.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="21.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="19.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="22.25"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="12" style="4" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2465,7 +2739,6 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>96</v>
       </c>
@@ -2498,7 +2771,6 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>106</v>
       </c>
@@ -2531,7 +2803,6 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
         <v>116</v>
       </c>
@@ -2564,7 +2835,6 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
         <v>126</v>
       </c>
@@ -2597,7 +2867,6 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
         <v>136</v>
       </c>
@@ -2630,7 +2899,6 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
         <v>146</v>
       </c>
@@ -2663,7 +2931,6 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
         <v>156</v>
       </c>
@@ -2696,8 +2963,6 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
         <v>166</v>
       </c>
@@ -2727,8 +2992,6 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
         <v>175</v>
       </c>
@@ -2758,249 +3021,208 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="D12" s="1"/>
+      <c r="D12" s="1" t="s">
+        <v>185</v>
+      </c>
       <c r="E12" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="D13" s="1"/>
+        <v>193</v>
+      </c>
       <c r="E13" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="D14" s="1"/>
+        <v>201</v>
+      </c>
       <c r="E14" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
+        <v>204</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>206</v>
+      </c>
       <c r="J14" s="1" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="D15" s="1"/>
+        <v>209</v>
+      </c>
       <c r="E15" s="1" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
+        <v>212</v>
+      </c>
       <c r="J15" s="1" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="D16" s="1"/>
+        <v>215</v>
+      </c>
       <c r="E16" s="1" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
+        <v>218</v>
+      </c>
       <c r="J16" s="1" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="D17" s="1"/>
+        <v>221</v>
+      </c>
       <c r="E17" s="1" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
+        <v>224</v>
+      </c>
       <c r="J17" s="5" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="K17" s="5" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="D18" s="1"/>
+        <v>227</v>
+      </c>
       <c r="E18" s="1" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>227</v>
-      </c>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
+        <v>230</v>
+      </c>
       <c r="J18" s="5" t="s">
-        <v>228</v>
-      </c>
-      <c r="K18" s="1"/>
+        <v>231</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>232</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="D19" s="1"/>
+        <v>233</v>
+      </c>
       <c r="E19" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
+        <v>234</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="D20" s="1"/>
+        <v>238</v>
+      </c>
       <c r="E20" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-    </row>
-    <row r="21" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
+        <v>239</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
+        <v>240</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
       <c r="C22" s="5" t="s">
-        <v>234</v>
-      </c>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
+        <v>242</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C23" s="1" t="s">
+        <v>243</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3026,176 +3248,176 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="33.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="43.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="33.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="6" width="43.93"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6" t="s">
-        <v>235</v>
+      <c r="A1" s="7" t="s">
+        <v>244</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>236</v>
+        <v>245</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
-        <v>237</v>
+      <c r="A2" s="8" t="s">
+        <v>246</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>238</v>
+        <v>247</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7" t="s">
-        <v>239</v>
+      <c r="A3" s="8" t="s">
+        <v>248</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>240</v>
+        <v>249</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="s">
-        <v>241</v>
+      <c r="A4" s="8" t="s">
+        <v>250</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>240</v>
+        <v>249</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="s">
-        <v>242</v>
+      <c r="A5" s="8" t="s">
+        <v>251</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>240</v>
+        <v>249</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7" t="s">
-        <v>243</v>
+      <c r="A6" s="8" t="s">
+        <v>252</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>244</v>
+        <v>253</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="7" t="s">
-        <v>245</v>
+      <c r="A7" s="8" t="s">
+        <v>254</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>244</v>
+        <v>253</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7" t="s">
-        <v>246</v>
+      <c r="A8" s="8" t="s">
+        <v>255</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7" t="s">
-        <v>248</v>
+      <c r="A9" s="8" t="s">
+        <v>257</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="7" t="s">
-        <v>249</v>
+      <c r="A10" s="8" t="s">
+        <v>258</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="7" t="s">
-        <v>250</v>
+      <c r="A11" s="8" t="s">
+        <v>259</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>251</v>
+        <v>260</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="7" t="s">
-        <v>252</v>
+      <c r="A12" s="8" t="s">
+        <v>261</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>251</v>
+        <v>260</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="7" t="n">
+      <c r="A13" s="8" t="n">
         <v>620050</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>251</v>
+        <v>260</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="7" t="n">
+      <c r="A14" s="8" t="n">
         <v>7708591995</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>251</v>
+        <v>260</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="7" t="s">
-        <v>253</v>
+      <c r="A15" s="8" t="s">
+        <v>262</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>251</v>
+        <v>260</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="7" t="s">
-        <v>254</v>
+      <c r="A16" s="8" t="s">
+        <v>263</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>255</v>
+        <v>264</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="7" t="s">
-        <v>256</v>
+      <c r="A17" s="8" t="s">
+        <v>265</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>257</v>
+        <v>266</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="7" t="s">
-        <v>258</v>
+      <c r="A18" s="8" t="s">
+        <v>267</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>259</v>
+        <v>268</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="7" t="s">
-        <v>260</v>
+      <c r="A19" s="8" t="s">
+        <v>269</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>261</v>
+        <v>270</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="7" t="s">
-        <v>262</v>
+      <c r="A20" s="8" t="s">
+        <v>271</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>263</v>
+        <v>272</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="7" t="s">
-        <v>264</v>
+      <c r="A21" s="8" t="s">
+        <v>273</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>265</v>
+        <v>274</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add: added taking the container number from the file and added folder handling
</commit_message>
<xml_diff>
--- a/unzipping_table.xlsx
+++ b/unzipping_table.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="labels_before_table" sheetId="1" state="visible" r:id="rId3"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="339">
   <si>
     <t xml:space="preserve">seller</t>
   </si>
@@ -39,6 +39,9 @@
     <t xml:space="preserve">destination_station</t>
   </si>
   <si>
+    <t xml:space="preserve">container_number</t>
+  </si>
+  <si>
     <t xml:space="preserve">SHIPPER/ГРУЗООТПРАВИТЕЛЬ</t>
   </si>
   <si>
@@ -182,6 +185,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">CONTAINER/КОНТЕЙНЕР</t>
+  </si>
+  <si>
     <t xml:space="preserve">THECONSIGNOR/ОТПРАВИТЕЛЬ</t>
   </si>
   <si>
@@ -231,6 +237,25 @@
     <t xml:space="preserve">PLACEOFDELIVERY/МЕСТОДОСТАВКИ</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">CONTAINER/КОНТЕЙНЕР/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">箱号</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">THESENDER/ОТПРАВИТЕЛЬ</t>
   </si>
   <si>
@@ -268,6 +293,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">买方）</t>
     </r>
@@ -346,6 +372,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">收货人及地址（添加运单第四栏公司和地址）</t>
     </r>
@@ -377,6 +404,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">买家</t>
     </r>
@@ -532,6 +560,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">目的地站</t>
     </r>
@@ -602,6 +631,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">目的站</t>
     </r>
@@ -636,6 +666,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">到达站</t>
     </r>
@@ -681,6 +712,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">目的站</t>
     </r>
@@ -752,6 +784,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">（发货人）</t>
     </r>
@@ -771,6 +804,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">卖方及地址</t>
     </r>
@@ -836,6 +870,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">发货人及地址（添加运单第一栏公司和地址）</t>
     </r>
@@ -861,6 +896,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">卖方</t>
     </r>
@@ -889,6 +925,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">买方及地址</t>
     </r>
@@ -1575,6 +1612,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">序号</t>
     </r>
@@ -1851,6 +1889,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">货源国</t>
     </r>
@@ -1928,6 +1967,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">货物原产国</t>
     </r>
@@ -2014,6 +2054,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">净重</t>
     </r>
@@ -2042,6 +2083,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">毛重</t>
     </r>
@@ -2088,6 +2130,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">净重</t>
     </r>
@@ -2105,6 +2148,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">千克</t>
     </r>
@@ -2124,6 +2168,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">毛重</t>
     </r>
@@ -2141,6 +2186,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">千克</t>
     </r>
@@ -2484,6 +2530,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">总价</t>
     </r>
@@ -2535,6 +2582,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">双数</t>
     </r>
@@ -2554,6 +2602,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">件数</t>
     </r>
@@ -2573,6 +2622,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">每双单价</t>
     </r>
@@ -2601,6 +2651,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">总价</t>
     </r>
@@ -2688,6 +2739,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">货物的最小单位数量</t>
     </r>
@@ -2707,6 +2759,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">外包装的数量</t>
     </r>
@@ -2726,6 +2779,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">每个货物最小单位的价格</t>
     </r>
@@ -2757,6 +2811,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">英俄文品名描述</t>
     </r>
@@ -2920,6 +2975,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">商编</t>
     </r>
@@ -2939,6 +2995,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">海关编码</t>
     </r>
@@ -2958,6 +3015,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">编码</t>
     </r>
@@ -3170,7 +3228,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3184,10 +3242,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3333,10 +3387,10 @@
   </sheetPr>
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
+      <selection pane="bottomLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3365,370 +3419,379 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="1" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="1" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -3749,7 +3812,7 @@
   </sheetPr>
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="K20" activeCellId="0" sqref="K20"/>
@@ -3773,659 +3836,659 @@
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="1" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="1" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="1" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="1" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="1" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="1" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="1" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="1" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>226</v>
+        <v>227</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>229</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="1" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>234</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>235</v>
+        <v>236</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>238</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="1" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="1" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="1" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="K16" s="5" t="s">
-        <v>262</v>
+        <v>264</v>
+      </c>
+      <c r="K16" s="4" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C17" s="1" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="J17" s="5" t="s">
-        <v>267</v>
-      </c>
-      <c r="K17" s="5" t="s">
-        <v>268</v>
+        <v>269</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C18" s="1" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>271</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>272</v>
-      </c>
-      <c r="J18" s="5" t="s">
         <v>273</v>
       </c>
+      <c r="F18" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>276</v>
+      </c>
       <c r="K18" s="1" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C19" s="1" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C20" s="1" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="1" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C22" s="5" t="s">
-        <v>292</v>
+      <c r="C22" s="4" t="s">
+        <v>295</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C23" s="1" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C24" s="1" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C25" s="1" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C26" s="1" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C27" s="1" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C28" s="5" t="s">
-        <v>299</v>
+      <c r="C28" s="4" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C29" s="1" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C30" s="1" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C31" s="1" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C32" s="1" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C33" s="1" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
     </row>
   </sheetData>
@@ -4454,176 +4517,176 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="33.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="6" width="43.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="5" width="33.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="5" width="43.93"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="7" t="s">
-        <v>305</v>
+      <c r="A1" s="6" t="s">
+        <v>308</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="s">
-        <v>307</v>
+      <c r="A2" s="7" t="s">
+        <v>310</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="s">
-        <v>309</v>
+      <c r="A3" s="7" t="s">
+        <v>312</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8" t="s">
-        <v>311</v>
+      <c r="A4" s="7" t="s">
+        <v>314</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8" t="s">
-        <v>312</v>
+      <c r="A5" s="7" t="s">
+        <v>315</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8" t="s">
-        <v>313</v>
+      <c r="A6" s="7" t="s">
+        <v>316</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="8" t="s">
-        <v>315</v>
+      <c r="A7" s="7" t="s">
+        <v>318</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8" t="s">
-        <v>316</v>
+      <c r="A8" s="7" t="s">
+        <v>319</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="8" t="s">
-        <v>318</v>
+      <c r="A9" s="7" t="s">
+        <v>321</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="8" t="s">
-        <v>319</v>
+      <c r="A10" s="7" t="s">
+        <v>322</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="8" t="s">
-        <v>320</v>
+      <c r="A11" s="7" t="s">
+        <v>323</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="8" t="s">
-        <v>322</v>
+      <c r="A12" s="7" t="s">
+        <v>325</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="8" t="n">
+      <c r="A13" s="7" t="n">
         <v>620050</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="8" t="n">
+      <c r="A14" s="7" t="n">
         <v>7708591995</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="8" t="s">
-        <v>323</v>
+      <c r="A15" s="7" t="s">
+        <v>326</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="8" t="s">
-        <v>324</v>
+      <c r="A16" s="7" t="s">
+        <v>327</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="8" t="s">
-        <v>326</v>
+      <c r="A17" s="7" t="s">
+        <v>329</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="8" t="s">
-        <v>328</v>
+      <c r="A18" s="7" t="s">
+        <v>331</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="8" t="s">
-        <v>330</v>
+      <c r="A19" s="7" t="s">
+        <v>333</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="8" t="s">
-        <v>332</v>
+      <c r="A20" s="7" t="s">
+        <v>335</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="8" t="s">
-        <v>334</v>
+      <c r="A21" s="7" t="s">
+        <v>337</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: change keys in table
</commit_message>
<xml_diff>
--- a/unzipping_table.xlsx
+++ b/unzipping_table.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="343">
   <si>
     <t xml:space="preserve">seller</t>
   </si>
@@ -48,53 +48,455 @@
     <t xml:space="preserve">CONSIGNOR/ГРУЗООТПРАВИТЕЛЬ/ПРОДАВЕЦ</t>
   </si>
   <si>
+    <t xml:space="preserve">ПОЛУЧАТЕЛЬ/CONSIGNEE</t>
+  </si>
+  <si>
     <t xml:space="preserve">ПОКУПАТЕЛЬ</t>
   </si>
   <si>
+    <t xml:space="preserve">BENEFICIARY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SHIPPER/ОТПРАВИТЕЛЬ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELLER</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ПОЛУЧАТЕЛЬ/CONSIGNEE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">收货人（与运单四栏公司一致）</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">ПОКУПАТЕЛЬ/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESTINATIONSTATION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SHIPPER/ОТПРАВИТЕЛЬ(SAMEASSMGS'SHIPPER)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELLER/SHIPPER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SHIPTO/ПОЛУЧАТЕЛЬ</t>
+  </si>
+  <si>
     <t xml:space="preserve">BUYER</t>
   </si>
   <si>
-    <t xml:space="preserve">BENEFICIARY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SHIPPER/ОТПРАВИТЕЛЬ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SELLER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ПОКУПАТЕЛЬ/</t>
+    <t xml:space="preserve">DESTINATIONSTATION/</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">SHIPPER/ОТПРАВИТЕЛЬ/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">发货人</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">SELLER/ПРОДАВЕЦ</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ПОКУПАТЕЛЬ(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">买方）</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">BUYER/</t>
   </si>
   <si>
-    <t xml:space="preserve">DESTINATIONSTATION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SHIPPER/ОТПРАВИТЕЛЬ(SAMEASSMGS'SHIPPER)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SELLER/SHIPPER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ПОЛУЧАТЕЛЬ/CONSIGNEE</t>
+    <t xml:space="preserve">DESTINATIONSTATION/СТАНЦИЯНАЗНАЧЕНИЯ</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">SHIPPER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">（发货人）</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">SELLER/ПРОДАВЕЦ/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ПОЛУЧАТЕЛЬ</t>
   </si>
   <si>
     <t xml:space="preserve">BUYER/CONSIGNEE</t>
   </si>
   <si>
-    <t xml:space="preserve">DESTINATIONSTATION/</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">SHIPPER/ОТПРАВИТЕЛЬ/</t>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">DESTINATIONSTATION/СТАНЦИЯНАЗНАЧЕНИЯ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">目的站</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">CONTAINER/КОНТЕЙНЕР</t>
+  </si>
+  <si>
+    <t xml:space="preserve">THECONSIGNOR/ОТПРАВИТЕЛЬ</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">SELLER/ПРОДАВЕЦ/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">卖家</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">ПОКУПАТЕЛЬСАДРЕСОМ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BUYER/ПОКУПАТЕЛЬ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PLACEOFDELIVERY/МЕСТОДОСТАВКИ</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">CONTAINER/КОНТЕЙНЕР/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">箱号</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">THESENDER/ОТПРАВИТЕЛЬ</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">SELLER/ПРОДАВЕЦ/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">卖方</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ПОЛУЧАТЕЛЬ/CONSIGNEE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">收货人及地址（添加运单第四栏公司和地址）</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">BUYER/ПОКУПАТЕЛЬ/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STATIONOFDESTINATION/СТАНЦИЯНАЗНАЧЕНИЯ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">КОНТЕЙНЕР/(CONTAINER)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">THESHIPPER/ОТПРАВИТЕЛЬ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SHIPPER/SELLER</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">BUYERПОКУПАТЕЛЬ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">买家</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">BUYER/ПОКУПАТЕЛЬ/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">买主</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">STATIONOFDESTINATIONСТАНЦИЯНАЗНАЧЕНИЯ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">НОМЕРКОНТЕЙНЕРА</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ГРУЗОТПРАВИТЕЛЬ/SHIPPER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">THESELLER/ПРОДАВЕЦ</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ПОКУПАТЕЛЬ/THEBUYER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">买方</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">BUYER/ПОКУПАТЕЛЬ/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">买方</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">СТАНЦИЯНАЗНАЧЕНИЯ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONTAINER/КОНТЕЙНЕРNO.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ОТПРАВИТЕЛЬ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ПРОДАВЕЦ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONSIGNEE/ГРУЗОПОЛУЧАТЕЛЬ/ПОКУПАТЕЛЬ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">СТАНЦИЯНАЗНАЧЕНИЯ(DESTINATIONSTATION)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONTAINER/КОНТЕЙНЕР/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ОТПРАВИТЕЛЬ/SHIPPER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ПРОДАВЕЦ/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">THEBUYER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">СТАНЦИЯНАЗНАЧЕНИЯ/DESTINATIONSTATION</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">CONTAINER/КОНТЕЙНЕР</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">箱号</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">ОТПРАВИТЕЛЬ/THESENDER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ПРОДАВЕЦ/SELLER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">THEBUYER/ПОКУПАТЕЛЬ</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">СТАНЦИЯНАЗНАЧЕНИЯ/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">目的车站</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ОТПРАВИТЕЛЬ/THESENDER</t>
     </r>
     <r>
       <rPr>
@@ -107,43 +509,302 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">SELLER/ПРОДАВЕЦ</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">ПОЛУЧАТЕЛЬ/CONSIGNEE</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">收货人（与运单四栏公司一致）</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">BUYER/ПОКУПАТЕЛЬ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DESTINATIONSTATION/СТАНЦИЯНАЗНАЧЕНИЯ</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">SHIPPER</t>
+    <t xml:space="preserve">ПРОДАВЕЦ/SELLERОТПРАВИТЕЛЬ/SENDER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">THEBUYER/ПОКУПАТЕЛЬTHECONSIGNEEE/ПОЛУЧАТЕЛЬ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">СТРАНАНАЗНАЧЕНИЯСТАНЦИЯНАЗНАЧЕНИЯ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ОТПРАВИТЕЛЬ/ПРОДАВЕЦ</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ПРОДАВЕЦ/SELLER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">卖家</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">ПОКУПАТЕЛЬ/BUYER</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">СТАНЦИЯНАЗНАЧЕНИЯ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">到站</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">ОТПРАВИТЕЛЬ/ПРОДАВЕЦSHIPPER/SELLER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ПРОДАВЕЦ/THESELLER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ПОКУПАТЕЛЬ/BUYERПОЛУЧАТЕЛЬ/RECIPIENT</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">СТАНЦИЯНАЗНАЧЕНИЯ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">目的地站</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ОТПРАВИТЕЛЬПОСТАНЦИИ/SHIPPERINSMGS/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">运单发货人</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ПРОДАВЕЦ/THESELLER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">卖方</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ПОКУПАТЕЛЬ/BUYER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">买家</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">目的站</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">/СТАНЦИЯНАЗНАЧЕНИЯ</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">ПРОДАВЕЦ/ОТПРАВИТЕЛЬ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ПОКУПАТЕЛЬ/THEBUYER</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">СТАНЦИЯПРИБЫТИЯ/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">到达站</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ОТПРАВИТЕЛЬ/SHIPPER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">发货人（与运单第一栏发货人一致）</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">ПРОДАВЕЦ/ОТПРАВИТЕЛЬSELLER/SHIPPER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ПОКУПАТЕЛЬ/ПОЛУЧАТЕЛЬ</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">СТАНЦИЯНАЗНАЧЕНИЯ/DESTINATIONSTATION/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">目的站</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">SHIPFROM/ОТПРАВИТЕЛЬ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ПРОДАВЕЦSELLER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ПОКУПАТЕЛЬBUYER</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ОТПРАВИТЕЛЬ/SHIPPER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">发货人</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ПРОДАВЕЦ/SELLER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">卖方</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">ПОЛУЧАТЕЛЬ/</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ОТПРАВИТЕЛЬ/ПРОДАВЕЦ</t>
     </r>
     <r>
       <rPr>
@@ -156,118 +817,106 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">SELLER/ПРОДАВЕЦ/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SHIPTO/ПОЛУЧАТЕЛЬ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BUYER/ПОКУПАТЕЛЬ/</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">DESTINATIONSTATION/СТАНЦИЯНАЗНАЧЕНИЯ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">目的站</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">CONTAINER/КОНТЕЙНЕР</t>
-  </si>
-  <si>
-    <t xml:space="preserve">THECONSIGNOR/ОТПРАВИТЕЛЬ</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">SELLER/ПРОДАВЕЦ/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">卖家</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">ПОЛУЧАТЕЛЬ/СONSIGNEE</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">BUYER/ПОКУПАТЕЛЬ/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">买主</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">PLACEOFDELIVERY/МЕСТОДОСТАВКИ</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">CONTAINER/КОНТЕЙНЕР/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">箱号</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">THESENDER/ОТПРАВИТЕЛЬ</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">SELLER/ПРОДАВЕЦ/</t>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ПРОДАВЕЦ/SELLER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">卖方及地址</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">ПОЛУЧАТЕЛЬ/ПОКУПАТЕЛЬ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ПРОДАВЕЦ/ОТПРАВИТЕЛЬСАДРЕСОМ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ОТПРАВИТЕЛЬ/SHIPPERПРОДАВЕЦ/SELLER</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ПОЛУЧАТЕЛЬ/THECONSIGNEE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">收货人</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ОТПРАВИТЕЛЬ/SHIPPER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">发货人及地址（添加运单第一栏公司和地址）</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">CONSIGNOR/ГРУЗООТПРАВИТЕЛЬ</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ПОКУПАТЕЛЬ/BUYER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">买方</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">SELLERПРОДАВЕЦ</t>
     </r>
     <r>
       <rPr>
@@ -280,272 +929,19 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">ПОКУПАТЕЛЬ(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">买方）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">BUYER/ПОКУПАТЕЛЬ/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">买方</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">STATIONOFDESTINATION/СТАНЦИЯНАЗНАЧЕНИЯ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">КОНТЕЙНЕР/(CONTAINER)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">THESHIPPER/ОТПРАВИТЕЛЬ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SHIPPER/SELLER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ПОЛУЧАТЕЛЬ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CONSIGNEE/ГРУЗОПОЛУЧАТЕЛЬ/ПОКУПАТЕЛЬ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STATIONOFDESTINATIONСТАНЦИЯНАЗНАЧЕНИЯ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">НОМЕРКОНТЕЙНЕРА</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ГРУЗОТПРАВИТЕЛЬ/SHIPPER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">THESELLER/ПРОДАВЕЦ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ПОКУПАТЕЛЬСАДРЕСОМ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">THEBUYER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">СТАНЦИЯНАЗНАЧЕНИЯ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CONTAINER/КОНТЕЙНЕРNO.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ОТПРАВИТЕЛЬ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ПРОДАВЕЦ</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">ПОЛУЧАТЕЛЬ/CONSIGNEE</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">收货人及地址（添加运单第四栏公司和地址）</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">THEBUYER/ПОКУПАТЕЛЬ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">СТАНЦИЯНАЗНАЧЕНИЯ(DESTINATIONSTATION)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CONTAINER/КОНТЕЙНЕР/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ОТПРАВИТЕЛЬ/SHIPPER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ПРОДАВЕЦ/</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">BUYERПОКУПАТЕЛЬ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">买家</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">THEBUYER/ПОКУПАТЕЛЬTHECONSIGNEEE/ПОЛУЧАТЕЛЬ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">СТАНЦИЯНАЗНАЧЕНИЯ/DESTINATIONSTATION</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">CONTAINER/КОНТЕЙНЕР</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">箱号</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">ОТПРАВИТЕЛЬ/THESENDER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ПРОДАВЕЦ/SELLER</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">ПОКУПАТЕЛЬ/THEBUYER</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">买方</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">ПОКУПАТЕЛЬ/BUYER</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">СТАНЦИЯНАЗНАЧЕНИЯ/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">目的车站</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">ОТПРАВИТЕЛЬ/THESENDER</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">发货人</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">ПРОДАВЕЦ/SELLERОТПРАВИТЕЛЬ/SENDER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ПОКУПАТЕЛЬ/BUYERПОЛУЧАТЕЛЬ/RECIPIENT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">СТРАНАНАЗНАЧЕНИЯСТАНЦИЯНАЗНАЧЕНИЯ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ОТПРАВИТЕЛЬ/ПРОДАВЕЦ</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">ПРОДАВЕЦ/SELLER</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">卖家</t>
-    </r>
+    <t xml:space="preserve">SHIPPER/ОТПРАВИТЕЛЬSELLER/ПРОДАВЕЦ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONSIGNEE/ГРУЗОПОЛУЧАТЕЛЬ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SHIPPER/SELLERОТПРАВИТЕЛЬ/ПРОДАВЕЦ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ПОКУПАТЕЛЬ/ПОЛУЧАТЕЛЬ/BUYER/CONSIGNEE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ОТПРАВИТЕЛЬ/ПРОДАВЕЦ/SHIPPER/SELLER</t>
   </si>
   <si>
     <r>
@@ -564,405 +960,8 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">买家</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">СТАНЦИЯНАЗНАЧЕНИЯ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">到站</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">ОТПРАВИТЕЛЬ/ПРОДАВЕЦSHIPPER/SELLER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ПРОДАВЕЦ/THESELLER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ПОКУПАТЕЛЬ/THEBUYER</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">СТАНЦИЯНАЗНАЧЕНИЯ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">目的地站</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">ОТПРАВИТЕЛЬПОСТАНЦИИ/SHIPPERINSMGS/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">运单发货人</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">ПРОДАВЕЦ/THESELLER</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">卖方</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">ПОКУПАТЕЛЬ/ПОЛУЧАТЕЛЬ</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">目的站</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">/СТАНЦИЯНАЗНАЧЕНИЯ</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">ПРОДАВЕЦ/ОТПРАВИТЕЛЬ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ПОКУПАТЕЛЬBUYER</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">СТАНЦИЯПРИБЫТИЯ/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">到达站</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">ОТПРАВИТЕЛЬ/SHIPPER</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">发货人（与运单第一栏发货人一致）</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">ПРОДАВЕЦ/ОТПРАВИТЕЛЬSELLER/SHIPPER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ПОЛУЧАТЕЛЬ/</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">СТАНЦИЯНАЗНАЧЕНИЯ/DESTINATIONSTATION/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">目的站</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">SHIPFROM/ОТПРАВИТЕЛЬ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ПРОДАВЕЦSELLER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ПОЛУЧАТЕЛЬ/ПОКУПАТЕЛЬ</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">ОТПРАВИТЕЛЬ/SHIPPER</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">发货人</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">ПРОДАВЕЦ/SELLER</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">卖方</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">ПОЛУЧАТЕЛЬ/THECONSIGNEE</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">收货人</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">ОТПРАВИТЕЛЬ/ПРОДАВЕЦ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">（发货人）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">ПРОДАВЕЦ/SELLER</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">卖方及地址</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">ПОКУПАТЕЛЬ/BUYER</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">买方</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">ПРОДАВЕЦ/ОТПРАВИТЕЛЬСАДРЕСОМ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ОТПРАВИТЕЛЬ/SHIPPERПРОДАВЕЦ/SELLER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CONSIGNEE/ГРУЗОПОЛУЧАТЕЛЬ</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">ОТПРАВИТЕЛЬ/SHIPPER</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">发货人及地址（添加运单第一栏公司和地址）</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">CONSIGNOR/ГРУЗООТПРАВИТЕЛЬ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ПОКУПАТЕЛЬ/ПОЛУЧАТЕЛЬ/BUYER/CONSIGNEE</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">SELLERПРОДАВЕЦ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">卖方</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">SHIPPER/ОТПРАВИТЕЛЬSELLER/ПРОДАВЕЦ</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">ПОКУПАТЕЛЬ/BUYER</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
       <t xml:space="preserve">买方及地址</t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">SHIPPER/SELLERОТПРАВИТЕЛЬ/ПРОДАВЕЦ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ОТПРАВИТЕЛЬ/ПРОДАВЕЦ/SHIPPER/SELLER</t>
   </si>
   <si>
     <t xml:space="preserve">model</t>
@@ -3152,7 +3151,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -3199,16 +3198,6 @@
       <name val="Noto Sans CJK SC"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <name val="Noto Sans CJK SC"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -3264,7 +3253,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3278,10 +3267,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3428,9 +3413,9 @@
   <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+      <selection pane="bottomLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3463,7 +3448,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" s="2" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -3479,8 +3464,9 @@
       <c r="E2" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" s="2" customFormat="true" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -3592,7 +3578,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>44</v>
       </c>
@@ -3612,7 +3598,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>50</v>
       </c>
@@ -3639,214 +3625,211 @@
       <c r="B11" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E17" s="4" t="s">
         <v>85</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="D26" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="D25" s="1" t="s">
+    </row>
+    <row r="27" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="1" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="26" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="1" t="s">
+      <c r="D27" s="1" t="s">
         <v>114</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="1" t="s">
-        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -3891,659 +3874,659 @@
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>125</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>146</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>156</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>166</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="K6" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="I7" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="J7" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="K7" s="1" t="s">
         <v>186</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="K8" s="1" t="s">
         <v>196</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="I9" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="J9" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="K9" s="1" t="s">
         <v>206</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="I10" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="J10" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="K10" s="1" t="s">
         <v>216</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="H11" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="I11" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="J11" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="K11" s="1" t="s">
         <v>226</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="H12" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="I12" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="I12" s="5" t="s">
+      <c r="J12" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="J12" s="1" t="s">
+      <c r="K12" s="1" t="s">
         <v>235</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="G13" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="H13" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="H13" s="5" t="s">
+      <c r="I13" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="I13" s="5" t="s">
+      <c r="J13" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="J13" s="1" t="s">
+      <c r="K13" s="1" t="s">
         <v>244</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="G14" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="H14" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="I14" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="I14" s="1" t="s">
+      <c r="J14" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="J14" s="1" t="s">
+      <c r="K14" s="1" t="s">
         <v>253</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="G15" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="H15" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="I15" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="I15" s="1" t="s">
+      <c r="J15" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="J15" s="1" t="s">
+      <c r="K15" s="1" t="s">
         <v>261</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="G16" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="H16" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="I16" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="I16" s="1" t="s">
+      <c r="J16" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="J16" s="1" t="s">
+      <c r="K16" s="4" t="s">
         <v>269</v>
-      </c>
-      <c r="K16" s="5" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C17" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="F17" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="G17" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="J17" s="4" t="s">
         <v>274</v>
       </c>
-      <c r="J17" s="5" t="s">
+      <c r="K17" s="4" t="s">
         <v>275</v>
-      </c>
-      <c r="K17" s="5" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C18" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="F18" s="4" t="s">
         <v>278</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="G18" s="4" t="s">
         <v>279</v>
       </c>
-      <c r="G18" s="5" t="s">
+      <c r="J18" s="4" t="s">
         <v>280</v>
       </c>
-      <c r="J18" s="5" t="s">
+      <c r="K18" s="1" t="s">
         <v>281</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C19" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="F19" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="G19" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="J19" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="J19" s="1" t="s">
+      <c r="K19" s="1" t="s">
         <v>287</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C20" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="G20" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="J20" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="J20" s="1" t="s">
+      <c r="K20" s="1" t="s">
         <v>293</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="F21" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="G21" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="G21" s="1" t="s">
+      <c r="J21" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="J21" s="1" t="s">
+    </row>
+    <row r="22" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C22" s="4" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="22" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C22" s="5" t="s">
+      <c r="E22" s="1" t="s">
         <v>300</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C23" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C24" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C25" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C26" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C27" s="1" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C28" s="4" t="s">
         <v>306</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C28" s="5" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C29" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C30" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C31" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C32" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C33" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
   </sheetData>
@@ -4572,176 +4555,176 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="33.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="6" width="43.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="5" width="33.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="5" width="43.93"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
+        <v>312</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="B1" s="2" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="7" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="s">
+      <c r="B2" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="B2" s="1" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="7" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="s">
+      <c r="B3" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="B3" s="1" t="s">
+    </row>
+    <row r="4" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="7" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8" t="s">
+      <c r="B4" s="1" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="7" t="s">
         <v>319</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8" t="s">
+      <c r="B5" s="1" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="7" t="s">
         <v>320</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8" t="s">
+      <c r="B6" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="B6" s="1" t="s">
+    </row>
+    <row r="7" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="7" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="8" t="s">
+      <c r="B7" s="1" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="7" t="s">
         <v>323</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8" t="s">
+      <c r="B8" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="B8" s="1" t="s">
+    </row>
+    <row r="9" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="7" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="8" t="s">
+      <c r="B9" s="1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="7" t="s">
         <v>326</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="8" t="s">
+      <c r="B10" s="1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="7" t="s">
         <v>327</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="8" t="s">
+      <c r="B11" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="B11" s="1" t="s">
+    </row>
+    <row r="12" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="7" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="8" t="s">
+      <c r="B12" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="7" t="n">
+        <v>620050</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="7" t="n">
+        <v>7708591995</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="7" t="s">
         <v>330</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="8" t="n">
-        <v>620050</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="8" t="n">
-        <v>7708591995</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="8" t="s">
+      <c r="B15" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="7" t="s">
         <v>331</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="8" t="s">
+      <c r="B16" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="B16" s="1" t="s">
+    </row>
+    <row r="17" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="7" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="8" t="s">
+      <c r="B17" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="B17" s="1" t="s">
+    </row>
+    <row r="18" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="7" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="8" t="s">
+      <c r="B18" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="B18" s="1" t="s">
+    </row>
+    <row r="19" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="7" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="8" t="s">
+      <c r="B19" s="1" t="s">
         <v>338</v>
       </c>
-      <c r="B19" s="1" t="s">
+    </row>
+    <row r="20" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="7" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="8" t="s">
+      <c r="B20" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="B20" s="1" t="s">
+    </row>
+    <row r="21" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="7" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="8" t="s">
+      <c r="B21" s="1" t="s">
         <v>342</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>343</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: changed keys in table
</commit_message>
<xml_diff>
--- a/unzipping_table.xlsx
+++ b/unzipping_table.xlsx
@@ -48,53 +48,458 @@
     <t xml:space="preserve">CONSIGNOR/ГРУЗООТПРАВИТЕЛЬ/ПРОДАВЕЦ</t>
   </si>
   <si>
+    <t xml:space="preserve">ПОЛУЧАТЕЛЬ/CONSIGNEE</t>
+  </si>
+  <si>
     <t xml:space="preserve">ПОКУПАТЕЛЬ</t>
   </si>
   <si>
+    <t xml:space="preserve">BENEFICIARY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SHIPPER/ОТПРАВИТЕЛЬ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELLER</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ПОЛУЧАТЕЛЬ/CONSIGNEE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">收货人（与运单四栏公司一致）</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">ПОКУПАТЕЛЬ/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESTINATIONSTATION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SHIPPER/ОТПРАВИТЕЛЬ(SAMEASSMGS'SHIPPER)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELLER/SHIPPER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SHIPTO/ПОЛУЧАТЕЛЬ</t>
+  </si>
+  <si>
     <t xml:space="preserve">BUYER</t>
   </si>
   <si>
-    <t xml:space="preserve">BENEFICIARY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SHIPPER/ОТПРАВИТЕЛЬ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SELLER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ПОКУПАТЕЛЬ/</t>
+    <t xml:space="preserve">DESTINATIONSTATION/</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">SHIPPER/ОТПРАВИТЕЛЬ/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">发货人</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">SELLER/ПРОДАВЕЦ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ПОЛУЧАТЕЛЬ/СONSIGNEE</t>
   </si>
   <si>
     <t xml:space="preserve">BUYER/</t>
   </si>
   <si>
-    <t xml:space="preserve">DESTINATIONSTATION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SHIPPER/ОТПРАВИТЕЛЬ(SAMEASSMGS'SHIPPER)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SELLER/SHIPPER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ПОЛУЧАТЕЛЬ/CONSIGNEE</t>
+    <t xml:space="preserve">DESTINATIONSTATION/СТАНЦИЯНАЗНАЧЕНИЯ</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">SHIPPER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">（发货人）</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">SELLER/ПРОДАВЕЦ/</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ПОКУПАТЕЛЬ(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">买方）</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">BUYER/CONSIGNEE</t>
   </si>
   <si>
-    <t xml:space="preserve">DESTINATIONSTATION/</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">SHIPPER/ОТПРАВИТЕЛЬ/</t>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">DESTINATIONSTATION/СТАНЦИЯНАЗНАЧЕНИЯ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">目的站</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">CONTAINER/КОНТЕЙНЕР</t>
+  </si>
+  <si>
+    <t xml:space="preserve">THECONSIGNOR/ОТПРАВИТЕЛЬ</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">SELLER/ПРОДАВЕЦ/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">卖家</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">ПОЛУЧАТЕЛЬ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BUYER/ПОКУПАТЕЛЬ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PLACEOFDELIVERY/МЕСТОДОСТАВКИ</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">CONTAINER/КОНТЕЙНЕР/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">箱号</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">THESENDER/ОТПРАВИТЕЛЬ</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">SELLER/ПРОДАВЕЦ/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">卖方</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">ПОКУПАТЕЛЬСАДРЕСОМ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BUYER/ПОКУПАТЕЛЬ/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STATIONOFDESTINATION/СТАНЦИЯНАЗНАЧЕНИЯ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">КОНТЕЙНЕР/(CONTAINER)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">THESHIPPER/ОТПРАВИТЕЛЬ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SHIPPER/SELLER</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ПОЛУЧАТЕЛЬ/CONSIGNEE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">收货人及地址（添加运单第四栏公司和地址）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">BUYER/ПОКУПАТЕЛЬ/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">买主</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">STATIONOFDESTINATIONСТАНЦИЯНАЗНАЧЕНИЯ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">НОМЕРКОНТЕЙНЕРА</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ГРУЗОТПРАВИТЕЛЬ/SHIPPER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">THESELLER/ПРОДАВЕЦ</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">BUYERПОКУПАТЕЛЬ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">买家</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">BUYER/ПОКУПАТЕЛЬ/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">买方</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">СТАНЦИЯНАЗНАЧЕНИЯ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONTAINER/КОНТЕЙНЕРNO.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ОТПРАВИТЕЛЬ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ПРОДАВЕЦ</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ПОКУПАТЕЛЬ/THEBUYER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">买方</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">CONSIGNEE/ГРУЗОПОЛУЧАТЕЛЬ/ПОКУПАТЕЛЬ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">СТАНЦИЯНАЗНАЧЕНИЯ(DESTINATIONSTATION)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONTAINER/КОНТЕЙНЕР/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ОТПРАВИТЕЛЬ/SHIPPER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ПРОДАВЕЦ/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">THEBUYER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">СТАНЦИЯНАЗНАЧЕНИЯ/DESTINATIONSTATION</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">CONTAINER/КОНТЕЙНЕР</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">箱号</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">ОТПРАВИТЕЛЬ/THESENDER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ПРОДАВЕЦ/SELLER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">THEBUYER/ПОКУПАТЕЛЬ</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">СТАНЦИЯНАЗНАЧЕНИЯ/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">目的车站</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ОТПРАВИТЕЛЬ/THESENDER</t>
     </r>
     <r>
       <rPr>
@@ -107,43 +512,302 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">SELLER/ПРОДАВЕЦ</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">ПОЛУЧАТЕЛЬ/CONSIGNEE</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">收货人（与运单四栏公司一致）</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">BUYER/ПОКУПАТЕЛЬ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DESTINATIONSTATION/СТАНЦИЯНАЗНАЧЕНИЯ</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">SHIPPER</t>
+    <t xml:space="preserve">ПРОДАВЕЦ/SELLERОТПРАВИТЕЛЬ/SENDER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">THEBUYER/ПОКУПАТЕЛЬTHECONSIGNEEE/ПОЛУЧАТЕЛЬ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">СТРАНАНАЗНАЧЕНИЯСТАНЦИЯНАЗНАЧЕНИЯ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ОТПРАВИТЕЛЬ/ПРОДАВЕЦ</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ПРОДАВЕЦ/SELLER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">卖家</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">ПОКУПАТЕЛЬ/BUYER</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">СТАНЦИЯНАЗНАЧЕНИЯ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">到站</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">ОТПРАВИТЕЛЬ/ПРОДАВЕЦSHIPPER/SELLER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ПРОДАВЕЦ/THESELLER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ПОКУПАТЕЛЬ/BUYERПОЛУЧАТЕЛЬ/RECIPIENT</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">СТАНЦИЯНАЗНАЧЕНИЯ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">目的地站</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ОТПРАВИТЕЛЬПОСТАНЦИИ/SHIPPERINSMGS/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">运单发货人</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ПРОДАВЕЦ/THESELLER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">卖方</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ПОКУПАТЕЛЬ/BUYER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">买家</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">目的站</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">/СТАНЦИЯНАЗНАЧЕНИЯ</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">ПРОДАВЕЦ/ОТПРАВИТЕЛЬ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ПОКУПАТЕЛЬ/THEBUYER</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">СТАНЦИЯПРИБЫТИЯ/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">到达站</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ОТПРАВИТЕЛЬ/SHIPPER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">发货人（与运单第一栏发货人一致）</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">ПРОДАВЕЦ/ОТПРАВИТЕЛЬSELLER/SHIPPER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ПОКУПАТЕЛЬ/ПОЛУЧАТЕЛЬ</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">СТАНЦИЯНАЗНАЧЕНИЯ/DESTINATIONSTATION/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">目的站</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">SHIPFROM/ОТПРАВИТЕЛЬ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ПРОДАВЕЦSELLER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ПОКУПАТЕЛЬBUYER</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ОТПРАВИТЕЛЬ/SHIPPER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">发货人</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ПРОДАВЕЦ/SELLER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">卖方</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">ПОЛУЧАТЕЛЬ/</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ОТПРАВИТЕЛЬ/ПРОДАВЕЦ</t>
     </r>
     <r>
       <rPr>
@@ -156,118 +820,106 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">SELLER/ПРОДАВЕЦ/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SHIPTO/ПОЛУЧАТЕЛЬ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BUYER/ПОКУПАТЕЛЬ/</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">DESTINATIONSTATION/СТАНЦИЯНАЗНАЧЕНИЯ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">目的站</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">CONTAINER/КОНТЕЙНЕР</t>
-  </si>
-  <si>
-    <t xml:space="preserve">THECONSIGNOR/ОТПРАВИТЕЛЬ</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">SELLER/ПРОДАВЕЦ/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">卖家</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">ПОЛУЧАТЕЛЬ/СONSIGNEE</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">BUYER/ПОКУПАТЕЛЬ/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">买主</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">PLACEOFDELIVERY/МЕСТОДОСТАВКИ</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">CONTAINER/КОНТЕЙНЕР/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">箱号</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">THESENDER/ОТПРАВИТЕЛЬ</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">SELLER/ПРОДАВЕЦ/</t>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ПРОДАВЕЦ/SELLER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">卖方及地址</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">ПОЛУЧАТЕЛЬ/ПОКУПАТЕЛЬ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ПРОДАВЕЦ/ОТПРАВИТЕЛЬСАДРЕСОМ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ОТПРАВИТЕЛЬ/SHIPPERПРОДАВЕЦ/SELLER</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ПОЛУЧАТЕЛЬ/THECONSIGNEE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">收货人</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ОТПРАВИТЕЛЬ/SHIPPER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">发货人及地址（添加运单第一栏公司和地址）</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">CONSIGNOR/ГРУЗООТПРАВИТЕЛЬ</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ПОКУПАТЕЛЬ/BUYER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">买方</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">SELLERПРОДАВЕЦ</t>
     </r>
     <r>
       <rPr>
@@ -280,272 +932,19 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">ПОКУПАТЕЛЬ(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">买方）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">BUYER/ПОКУПАТЕЛЬ/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">买方</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">STATIONOFDESTINATION/СТАНЦИЯНАЗНАЧЕНИЯ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">КОНТЕЙНЕР/(CONTAINER)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">THESHIPPER/ОТПРАВИТЕЛЬ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SHIPPER/SELLER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ПОЛУЧАТЕЛЬ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CONSIGNEE/ГРУЗОПОЛУЧАТЕЛЬ/ПОКУПАТЕЛЬ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STATIONOFDESTINATIONСТАНЦИЯНАЗНАЧЕНИЯ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">НОМЕРКОНТЕЙНЕРА</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ГРУЗОТПРАВИТЕЛЬ/SHIPPER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">THESELLER/ПРОДАВЕЦ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ПОКУПАТЕЛЬСАДРЕСОМ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">THEBUYER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">СТАНЦИЯНАЗНАЧЕНИЯ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CONTAINER/КОНТЕЙНЕРNO.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ОТПРАВИТЕЛЬ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ПРОДАВЕЦ</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">ПОЛУЧАТЕЛЬ/CONSIGNEE</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">收货人及地址（添加运单第四栏公司和地址）</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">THEBUYER/ПОКУПАТЕЛЬ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">СТАНЦИЯНАЗНАЧЕНИЯ(DESTINATIONSTATION)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CONTAINER/КОНТЕЙНЕР/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ОТПРАВИТЕЛЬ/SHIPPER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ПРОДАВЕЦ/</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">BUYERПОКУПАТЕЛЬ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">买家</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">THEBUYER/ПОКУПАТЕЛЬTHECONSIGNEEE/ПОЛУЧАТЕЛЬ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">СТАНЦИЯНАЗНАЧЕНИЯ/DESTINATIONSTATION</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">CONTAINER/КОНТЕЙНЕР</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">箱号</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">ОТПРАВИТЕЛЬ/THESENDER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ПРОДАВЕЦ/SELLER</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">ПОКУПАТЕЛЬ/THEBUYER</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">买方</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">ПОКУПАТЕЛЬ/BUYER</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">СТАНЦИЯНАЗНАЧЕНИЯ/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">目的车站</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">ОТПРАВИТЕЛЬ/THESENDER</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">发货人</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">ПРОДАВЕЦ/SELLERОТПРАВИТЕЛЬ/SENDER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ПОКУПАТЕЛЬ/BUYERПОЛУЧАТЕЛЬ/RECIPIENT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">СТРАНАНАЗНАЧЕНИЯСТАНЦИЯНАЗНАЧЕНИЯ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ОТПРАВИТЕЛЬ/ПРОДАВЕЦ</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">ПРОДАВЕЦ/SELLER</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">卖家</t>
-    </r>
+    <t xml:space="preserve">SHIPPER/ОТПРАВИТЕЛЬSELLER/ПРОДАВЕЦ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONSIGNEE/ГРУЗОПОЛУЧАТЕЛЬ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SHIPPER/SELLERОТПРАВИТЕЛЬ/ПРОДАВЕЦ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ПОКУПАТЕЛЬ/ПОЛУЧАТЕЛЬ/BUYER/CONSIGNEE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ОТПРАВИТЕЛЬ/ПРОДАВЕЦ/SHIPPER/SELLER</t>
   </si>
   <si>
     <r>
@@ -564,405 +963,8 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">买家</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">СТАНЦИЯНАЗНАЧЕНИЯ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">到站</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">ОТПРАВИТЕЛЬ/ПРОДАВЕЦSHIPPER/SELLER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ПРОДАВЕЦ/THESELLER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ПОКУПАТЕЛЬ/THEBUYER</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">СТАНЦИЯНАЗНАЧЕНИЯ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">目的地站</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">ОТПРАВИТЕЛЬПОСТАНЦИИ/SHIPPERINSMGS/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">运单发货人</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">ПРОДАВЕЦ/THESELLER</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">卖方</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">ПОКУПАТЕЛЬ/ПОЛУЧАТЕЛЬ</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">目的站</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">/СТАНЦИЯНАЗНАЧЕНИЯ</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">ПРОДАВЕЦ/ОТПРАВИТЕЛЬ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ПОКУПАТЕЛЬBUYER</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">СТАНЦИЯПРИБЫТИЯ/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">到达站</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">ОТПРАВИТЕЛЬ/SHIPPER</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">发货人（与运单第一栏发货人一致）</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">ПРОДАВЕЦ/ОТПРАВИТЕЛЬSELLER/SHIPPER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ПОЛУЧАТЕЛЬ/</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">СТАНЦИЯНАЗНАЧЕНИЯ/DESTINATIONSTATION/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">目的站</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">SHIPFROM/ОТПРАВИТЕЛЬ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ПРОДАВЕЦSELLER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ПОЛУЧАТЕЛЬ/ПОКУПАТЕЛЬ</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">ОТПРАВИТЕЛЬ/SHIPPER</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">发货人</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">ПРОДАВЕЦ/SELLER</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">卖方</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">ПОЛУЧАТЕЛЬ/THECONSIGNEE</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">收货人</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">ОТПРАВИТЕЛЬ/ПРОДАВЕЦ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">（发货人）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">ПРОДАВЕЦ/SELLER</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">卖方及地址</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">ПОКУПАТЕЛЬ/BUYER</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">买方</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">ПРОДАВЕЦ/ОТПРАВИТЕЛЬСАДРЕСОМ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ОТПРАВИТЕЛЬ/SHIPPERПРОДАВЕЦ/SELLER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CONSIGNEE/ГРУЗОПОЛУЧАТЕЛЬ</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">ОТПРАВИТЕЛЬ/SHIPPER</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">发货人及地址（添加运单第一栏公司和地址）</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">CONSIGNOR/ГРУЗООТПРАВИТЕЛЬ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ПОКУПАТЕЛЬ/ПОЛУЧАТЕЛЬ/BUYER/CONSIGNEE</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">SELLERПРОДАВЕЦ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">卖方</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">SHIPPER/ОТПРАВИТЕЛЬSELLER/ПРОДАВЕЦ</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">ПОКУПАТЕЛЬ/BUYER</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
       <t xml:space="preserve">买方及地址</t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">SHIPPER/SELLERОТПРАВИТЕЛЬ/ПРОДАВЕЦ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ОТПРАВИТЕЛЬ/ПРОДАВЕЦ/SHIPPER/SELLER</t>
   </si>
   <si>
     <t xml:space="preserve">model</t>
@@ -3152,7 +3154,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -3199,16 +3201,6 @@
       <name val="Noto Sans CJK SC"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <name val="Noto Sans CJK SC"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -3264,7 +3256,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3278,10 +3270,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3428,9 +3416,9 @@
   <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+      <selection pane="bottomLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3463,7 +3451,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" s="2" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -3479,8 +3467,9 @@
       <c r="E2" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" s="2" customFormat="true" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -3592,7 +3581,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>44</v>
       </c>
@@ -3612,7 +3601,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>50</v>
       </c>
@@ -3659,193 +3648,193 @@
       <c r="B12" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="E13" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="E17" s="4" t="s">
         <v>86</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B25" s="1" t="s">
+    </row>
+    <row r="26" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D26" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="1" t="s">
+    <row r="27" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="1" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="27" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="1" t="s">
+      <c r="D27" s="1" t="s">
         <v>115</v>
       </c>
     </row>
@@ -4263,10 +4252,10 @@
       <c r="G12" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="H12" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="I12" s="5" t="s">
+      <c r="I12" s="4" t="s">
         <v>234</v>
       </c>
       <c r="J12" s="1" t="s">
@@ -4292,10 +4281,10 @@
       <c r="G13" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="H13" s="5" t="s">
+      <c r="H13" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="I13" s="5" t="s">
+      <c r="I13" s="4" t="s">
         <v>243</v>
       </c>
       <c r="J13" s="1" t="s">
@@ -4382,7 +4371,7 @@
       <c r="J16" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="K16" s="5" t="s">
+      <c r="K16" s="4" t="s">
         <v>270</v>
       </c>
     </row>
@@ -4399,10 +4388,10 @@
       <c r="G17" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="J17" s="5" t="s">
+      <c r="J17" s="4" t="s">
         <v>275</v>
       </c>
-      <c r="K17" s="5" t="s">
+      <c r="K17" s="4" t="s">
         <v>276</v>
       </c>
     </row>
@@ -4413,13 +4402,13 @@
       <c r="E18" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="F18" s="4" t="s">
         <v>279</v>
       </c>
-      <c r="G18" s="5" t="s">
+      <c r="G18" s="4" t="s">
         <v>280</v>
       </c>
-      <c r="J18" s="5" t="s">
+      <c r="J18" s="4" t="s">
         <v>281</v>
       </c>
       <c r="K18" s="1" t="s">
@@ -4484,7 +4473,7 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="4" t="s">
         <v>300</v>
       </c>
       <c r="E22" s="1" t="s">
@@ -4517,7 +4506,7 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="4" t="s">
         <v>307</v>
       </c>
     </row>
@@ -4572,12 +4561,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="33.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="6" width="43.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="5" width="33.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="5" width="43.93"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>313</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -4585,7 +4574,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>315</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -4593,7 +4582,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>317</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -4601,7 +4590,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>319</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -4609,7 +4598,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>320</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -4617,7 +4606,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>321</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -4625,7 +4614,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="7" t="s">
         <v>323</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -4633,7 +4622,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="7" t="s">
         <v>324</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -4641,7 +4630,7 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="7" t="s">
         <v>326</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -4649,7 +4638,7 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="7" t="s">
         <v>327</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -4657,7 +4646,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="7" t="s">
         <v>328</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -4665,7 +4654,7 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="7" t="s">
         <v>330</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -4673,7 +4662,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="8" t="n">
+      <c r="A13" s="7" t="n">
         <v>620050</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -4681,7 +4670,7 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="8" t="n">
+      <c r="A14" s="7" t="n">
         <v>7708591995</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -4689,7 +4678,7 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="7" t="s">
         <v>331</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -4697,7 +4686,7 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="7" t="s">
         <v>332</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -4705,7 +4694,7 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="7" t="s">
         <v>334</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -4713,7 +4702,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="7" t="s">
         <v>336</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -4721,7 +4710,7 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="7" t="s">
         <v>338</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -4729,7 +4718,7 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="8" t="s">
+      <c r="A20" s="7" t="s">
         <v>340</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -4737,7 +4726,7 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="7" t="s">
         <v>342</v>
       </c>
       <c r="B21" s="1" t="s">

</xml_diff>

<commit_message>
add: search inn in sheet xlsx and merge cells
</commit_message>
<xml_diff>
--- a/unzipping_table.xlsx
+++ b/unzipping_table.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="365">
   <si>
     <t xml:space="preserve">seller</t>
   </si>
@@ -973,6 +973,25 @@
   </si>
   <si>
     <t xml:space="preserve">СТАНЦИЯНАЗНАЧЕНИЯDESTINATIONSTATION</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ОТПРАВИТЕЛЬ/THESHIPPER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">发货人</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">SHIPPER/ОТПРАВИТЕЛЬSELLER/ПРОДАВЕЦ</t>
@@ -3614,7 +3633,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -3661,6 +3680,11 @@
       <name val="Noto Sans CJK SC"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="Noto Sans CJK SC"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -3872,7 +3896,7 @@
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
     </sheetView>
@@ -4273,40 +4297,43 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>113</v>
+      </c>
       <c r="B24" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>33</v>
@@ -4317,42 +4344,42 @@
         <v>90</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -4376,7 +4403,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C38" activeCellId="1" sqref="A24 C38"/>
+      <selection pane="bottomLeft" activeCell="C38" activeCellId="0" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4397,687 +4424,687 @@
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C17" s="1" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C18" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C19" s="1" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C20" s="1" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="1" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C22" s="3" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C23" s="1" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C24" s="1" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C25" s="1" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C26" s="1" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C27" s="1" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C28" s="3" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C29" s="1" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C30" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C31" s="1" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C32" s="1" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C33" s="1" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="1" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C35" s="1" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C36" s="1" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C37" s="1" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C38" s="1" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
   </sheetData>
@@ -5101,7 +5128,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B10" activeCellId="1" sqref="A24 B10"/>
+      <selection pane="bottomLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5112,98 +5139,98 @@
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
+        <v>340</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>339</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>343</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
+        <v>347</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>346</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
+        <v>351</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>350</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5211,7 +5238,7 @@
         <v>620050</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5219,63 +5246,63 @@
         <v>7708591995</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="6" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="6" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add: added new column name
</commit_message>
<xml_diff>
--- a/unzipping_table.xlsx
+++ b/unzipping_table.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="365">
   <si>
     <t xml:space="preserve">seller</t>
   </si>
@@ -973,6 +973,25 @@
   </si>
   <si>
     <t xml:space="preserve">СТАНЦИЯНАЗНАЧЕНИЯDESTINATIONSTATION</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ОТПРАВИТЕЛЬ/THESHIPPER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">发货人</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">SHIPPER/ОТПРАВИТЕЛЬSELLER/ПРОДАВЕЦ</t>
@@ -3614,7 +3633,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -3661,6 +3680,11 @@
       <name val="Noto Sans CJK SC"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="Noto Sans CJK SC"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -4273,40 +4297,43 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>113</v>
+      </c>
       <c r="B24" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>33</v>
@@ -4317,42 +4344,42 @@
         <v>90</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -4376,7 +4403,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C38" activeCellId="1" sqref="A24 C38"/>
+      <selection pane="bottomLeft" activeCell="C38" activeCellId="0" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4397,687 +4424,687 @@
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C17" s="1" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C18" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C19" s="1" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C20" s="1" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="1" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C22" s="3" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C23" s="1" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C24" s="1" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C25" s="1" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C26" s="1" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C27" s="1" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C28" s="3" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C29" s="1" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C30" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C31" s="1" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C32" s="1" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C33" s="1" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="1" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C35" s="1" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C36" s="1" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C37" s="1" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C38" s="1" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
   </sheetData>
@@ -5101,7 +5128,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B10" activeCellId="1" sqref="A24 B10"/>
+      <selection pane="bottomLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5112,98 +5139,98 @@
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
+        <v>340</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>339</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>343</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
+        <v>347</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>346</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
+        <v>351</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>350</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5211,7 +5238,7 @@
         <v>620050</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5219,63 +5246,63 @@
         <v>7708591995</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="6" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="6" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add: added parsing data by length of content data
</commit_message>
<xml_diff>
--- a/unzipping_table.xlsx
+++ b/unzipping_table.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="376">
   <si>
     <t xml:space="preserve">seller</t>
   </si>
@@ -989,6 +989,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">发货人</t>
     </r>
@@ -1017,6 +1018,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">СТАНЦИЯ</t>
+  </si>
+  <si>
     <t xml:space="preserve">SHIPPER/SELLERОТПРАВИТЕЛЬ/ПРОДАВЕЦ</t>
   </si>
   <si>
@@ -1095,6 +1099,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">BUYERПОКУПАТЕЛЬ</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="14"/>
@@ -1271,6 +1278,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">SHIPPERОТПРАВИТЕЛЬ/SELLERПРОДАВЕЦ</t>
+  </si>
+  <si>
     <t xml:space="preserve">model</t>
   </si>
   <si>
@@ -2368,6 +2378,9 @@
     <t xml:space="preserve">HSCODEГНГ</t>
   </si>
   <si>
+    <t xml:space="preserve">ORIGINCOUNTRY/СТРАНАПРОИСХОЖД</t>
+  </si>
+  <si>
     <t xml:space="preserve">ОПИСАНИЕТОВАРОВ</t>
   </si>
   <si>
@@ -2581,6 +2594,12 @@
     <t xml:space="preserve">КОЛИЧЕСТВОШТУК</t>
   </si>
   <si>
+    <t xml:space="preserve">TOTALN.W.(KGS)/НЕТТО,КГ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOTALG.W.(KGS)/БРУТТО,КГ</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="14"/>
@@ -3131,6 +3150,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">TOTALAMOUNT(CNY)/ОБЩАЯСТОИМОСТЬ,ЮАНЬ</t>
+  </si>
+  <si>
     <t xml:space="preserve">（清关HS编码）HSCODE/КОДТНВЭДТС</t>
   </si>
   <si>
@@ -3154,6 +3176,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">QTY(PCS)/КОЛ-ВО(ШТ)</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="14"/>
@@ -3250,6 +3275,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">PRODUCTDESCRIPTION/ОПИСАНИЕТОВАРА.</t>
+  </si>
+  <si>
     <t xml:space="preserve">CUSTOMSCOMMODITYCODE</t>
   </si>
   <si>
@@ -3531,6 +3559,12 @@
       </rPr>
       <t xml:space="preserve">编码</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">HSCODE/КОДТНВЭДТС/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HSCODE/ТНВЭДТС</t>
   </si>
   <si>
     <t xml:space="preserve">station</t>
@@ -3683,7 +3717,7 @@
     </font>
     <font>
       <sz val="14"/>
-      <name val="Noto Sans CJK SC"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -3740,7 +3774,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3754,6 +3788,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3893,12 +3931,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
+      <selection pane="bottomLeft" activeCell="D30" activeCellId="0" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4306,34 +4344,37 @@
       <c r="D24" s="1" t="s">
         <v>115</v>
       </c>
+      <c r="E24" s="4" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>33</v>
@@ -4344,42 +4385,50 @@
         <v>90</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="1" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="1" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="1" t="s">
-        <v>130</v>
+        <v>132</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="1" t="s">
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -4387,8 +4436,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Обычный"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Обычный"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -4398,12 +4447,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K38"/>
+  <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C38" activeCellId="0" sqref="C38"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="K21" activeCellId="0" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4424,687 +4473,715 @@
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="1" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="1" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="1" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="1" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="1" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="1" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="1" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="1" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="1" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="1" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="1" t="s">
-        <v>270</v>
+        <v>273</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>274</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="1" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C17" s="1" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>289</v>
+        <v>293</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>295</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>290</v>
+        <v>296</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>291</v>
+        <v>297</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C18" s="1" t="s">
-        <v>292</v>
+        <v>298</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>293</v>
+        <v>299</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>294</v>
+        <v>300</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>295</v>
+        <v>301</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>296</v>
+        <v>302</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>297</v>
+        <v>303</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C19" s="1" t="s">
-        <v>298</v>
+        <v>304</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>299</v>
+        <v>305</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>300</v>
+        <v>306</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>301</v>
+        <v>307</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>302</v>
+        <v>308</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>303</v>
+        <v>309</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C20" s="1" t="s">
-        <v>304</v>
+        <v>310</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>305</v>
+        <v>311</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>306</v>
+        <v>312</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>307</v>
+        <v>313</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>308</v>
+        <v>314</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>309</v>
+        <v>315</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="1" t="s">
-        <v>310</v>
+        <v>316</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>311</v>
+        <v>317</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>312</v>
+        <v>318</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>313</v>
+        <v>319</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>314</v>
+        <v>320</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C22" s="3" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>316</v>
+        <v>323</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C23" s="1" t="s">
-        <v>317</v>
+        <v>325</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>318</v>
+        <v>326</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C24" s="1" t="s">
-        <v>319</v>
+        <v>327</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>328</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C25" s="1" t="s">
-        <v>320</v>
+        <v>329</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C26" s="1" t="s">
-        <v>321</v>
+        <v>330</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C27" s="1" t="s">
-        <v>322</v>
+        <v>331</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C28" s="3" t="s">
-        <v>323</v>
+        <v>332</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C29" s="1" t="s">
-        <v>324</v>
+        <v>333</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C30" s="1" t="s">
-        <v>325</v>
+        <v>334</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C31" s="1" t="s">
-        <v>326</v>
+        <v>335</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C32" s="1" t="s">
-        <v>327</v>
+        <v>336</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C33" s="1" t="s">
-        <v>328</v>
+        <v>337</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="1" t="s">
-        <v>329</v>
+        <v>338</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C35" s="1" t="s">
-        <v>330</v>
+        <v>339</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C36" s="1" t="s">
-        <v>331</v>
+        <v>340</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C37" s="1" t="s">
-        <v>332</v>
+        <v>341</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C38" s="1" t="s">
-        <v>333</v>
+        <v>342</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C39" s="1" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C40" s="1" t="s">
+        <v>344</v>
       </c>
     </row>
   </sheetData>
@@ -5112,8 +5189,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Обычный"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Обычный"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -5133,176 +5210,176 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="33.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="43.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="5" width="33.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="5" width="43.93"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
-        <v>334</v>
+      <c r="A1" s="6" t="s">
+        <v>345</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>335</v>
+        <v>346</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
-        <v>336</v>
+      <c r="A2" s="7" t="s">
+        <v>347</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>337</v>
+        <v>348</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
-        <v>338</v>
+      <c r="A3" s="7" t="s">
+        <v>349</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>339</v>
+        <v>350</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="s">
-        <v>340</v>
+      <c r="A4" s="7" t="s">
+        <v>351</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>339</v>
+        <v>350</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="s">
-        <v>341</v>
+      <c r="A5" s="7" t="s">
+        <v>352</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>339</v>
+        <v>350</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6" t="s">
-        <v>342</v>
+      <c r="A6" s="7" t="s">
+        <v>353</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>343</v>
+        <v>354</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6" t="s">
-        <v>344</v>
+      <c r="A7" s="7" t="s">
+        <v>355</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>343</v>
+        <v>354</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6" t="s">
-        <v>345</v>
+      <c r="A8" s="7" t="s">
+        <v>356</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>346</v>
+        <v>357</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6" t="s">
-        <v>347</v>
+      <c r="A9" s="7" t="s">
+        <v>358</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>346</v>
+        <v>357</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="6" t="s">
-        <v>348</v>
+      <c r="A10" s="7" t="s">
+        <v>359</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>346</v>
+        <v>357</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="6" t="s">
-        <v>349</v>
+      <c r="A11" s="7" t="s">
+        <v>360</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>350</v>
+        <v>361</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="6" t="s">
-        <v>351</v>
+      <c r="A12" s="7" t="s">
+        <v>362</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>350</v>
+        <v>361</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="6" t="n">
+      <c r="A13" s="7" t="n">
         <v>620050</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>350</v>
+        <v>361</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="6" t="n">
+      <c r="A14" s="7" t="n">
         <v>7708591995</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>350</v>
+        <v>361</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="6" t="s">
-        <v>352</v>
+      <c r="A15" s="7" t="s">
+        <v>363</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>350</v>
+        <v>361</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="6" t="s">
-        <v>353</v>
+      <c r="A16" s="7" t="s">
+        <v>364</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>354</v>
+        <v>365</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="6" t="s">
-        <v>355</v>
+      <c r="A17" s="7" t="s">
+        <v>366</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>356</v>
+        <v>367</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="6" t="s">
-        <v>357</v>
+      <c r="A18" s="7" t="s">
+        <v>368</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>358</v>
+        <v>369</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="6" t="s">
-        <v>359</v>
+      <c r="A19" s="7" t="s">
+        <v>370</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>360</v>
+        <v>371</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="6" t="s">
-        <v>361</v>
+      <c r="A20" s="7" t="s">
+        <v>372</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>362</v>
+        <v>373</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="6" t="s">
-        <v>363</v>
+      <c r="A21" s="7" t="s">
+        <v>374</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>364</v>
+        <v>375</v>
       </c>
     </row>
   </sheetData>
@@ -5310,8 +5387,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Обычный"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Обычный"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add: added new archive 7z
</commit_message>
<xml_diff>
--- a/unzipping_table.xlsx
+++ b/unzipping_table.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="386">
   <si>
     <t xml:space="preserve">seller</t>
   </si>
@@ -572,6 +572,9 @@
     <t xml:space="preserve">ПРОДАВЕЦ/SELLERОТПРАВИТЕЛЬ/SENDER</t>
   </si>
   <si>
+    <t xml:space="preserve">ИЗГОТОВИТЕЛЬ/MANUFACTURER</t>
+  </si>
+  <si>
     <t xml:space="preserve">THEBUYER</t>
   </si>
   <si>
@@ -1027,6 +1030,9 @@
     <t xml:space="preserve">ПОКУПАТЕЛЬ/ПОЛУЧАТЕЛЬ/BUYER/CONSIGNEE</t>
   </si>
   <si>
+    <t xml:space="preserve">STATIONOFDESTINATION</t>
+  </si>
+  <si>
     <t xml:space="preserve">ОТПРАВИТЕЛЬ/ПРОДАВЕЦ/SHIPPER/SELLER</t>
   </si>
   <si>
@@ -1373,6 +1379,9 @@
     <t xml:space="preserve">AMOUNT(USD)</t>
   </si>
   <si>
+    <t xml:space="preserve">MODEL/МОДЕЛЬ</t>
+  </si>
+  <si>
     <t xml:space="preserve">NO.</t>
   </si>
   <si>
@@ -2686,6 +2695,12 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">N.WKGS/ОБЩИЙВЕСНЕТТОКГ.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G.W.KGS/ОБЩИЙВЕСБРУТТОКГ.</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="14"/>
@@ -3179,6 +3194,15 @@
     <t xml:space="preserve">QTY(PCS)/КОЛ-ВО(ШТ)</t>
   </si>
   <si>
+    <t xml:space="preserve">PACKING/КОЛИЧЕСТВОГРУЗОВЫХМЕСТ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRICE/ЦЕНА</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOTAL/ОБЩЕЕ</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="14"/>
@@ -3255,6 +3279,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">QUANTITY/КОЛИЧЕСТВОШТУК</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="14"/>
@@ -3279,6 +3306,9 @@
   </si>
   <si>
     <t xml:space="preserve">CUSTOMSCOMMODITYCODE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESCRIPTION/ОПИСАНИЕ</t>
   </si>
   <si>
     <t xml:space="preserve">CUSTOMSCOD/КОДТНВЭД</t>
@@ -3667,7 +3697,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -3714,11 +3744,6 @@
       <name val="Noto Sans CJK SC"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -3774,7 +3799,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3788,10 +3813,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3934,9 +3955,9 @@
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D30" activeCellId="0" sqref="D30"/>
+      <selection pane="bottomLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4201,180 +4222,186 @@
       <c r="B14" s="1" t="s">
         <v>74</v>
       </c>
+      <c r="C14" s="1" t="s">
+        <v>75</v>
+      </c>
       <c r="D14" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="E24" s="4" t="s">
         <v>116</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>33</v>
@@ -4382,53 +4409,53 @@
     </row>
     <row r="29" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="1" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="1" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="1" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="1" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="1" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="1" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -4449,10 +4476,10 @@
   </sheetPr>
   <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="K21" activeCellId="0" sqref="K21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="K22" activeCellId="0" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4473,715 +4500,739 @@
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>158</v>
+      </c>
       <c r="B3" s="1" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="1" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="1" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="1" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="1" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="1" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="1" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="1" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="1" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="1" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="1" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="1" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C17" s="1" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C18" s="1" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>301</v>
+        <v>304</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>306</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>302</v>
+        <v>307</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>303</v>
+        <v>308</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C19" s="1" t="s">
-        <v>304</v>
+        <v>309</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>306</v>
+        <v>311</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>307</v>
+        <v>312</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>308</v>
+        <v>313</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>309</v>
+        <v>314</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C20" s="1" t="s">
-        <v>310</v>
+        <v>315</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>311</v>
+        <v>316</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>312</v>
+        <v>317</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>315</v>
+        <v>320</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="1" t="s">
-        <v>316</v>
+        <v>321</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>317</v>
+        <v>322</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>318</v>
+        <v>323</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>319</v>
+        <v>324</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>320</v>
+        <v>325</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>321</v>
+        <v>326</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C22" s="3" t="s">
-        <v>322</v>
+        <v>327</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>323</v>
+        <v>328</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>324</v>
+        <v>329</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C23" s="1" t="s">
-        <v>325</v>
+        <v>333</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>326</v>
+        <v>334</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C24" s="1" t="s">
-        <v>327</v>
+        <v>336</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>328</v>
+        <v>337</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C25" s="1" t="s">
-        <v>329</v>
+        <v>338</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>339</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C26" s="1" t="s">
-        <v>330</v>
+        <v>340</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C27" s="1" t="s">
-        <v>331</v>
+        <v>341</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C28" s="3" t="s">
-        <v>332</v>
+        <v>342</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C29" s="1" t="s">
-        <v>333</v>
+        <v>343</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C30" s="1" t="s">
-        <v>334</v>
+        <v>344</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C31" s="1" t="s">
-        <v>335</v>
+        <v>345</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C32" s="1" t="s">
-        <v>336</v>
+        <v>346</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C33" s="1" t="s">
-        <v>337</v>
+        <v>347</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="1" t="s">
-        <v>338</v>
+        <v>348</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C35" s="1" t="s">
-        <v>339</v>
+        <v>349</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C36" s="1" t="s">
-        <v>340</v>
+        <v>350</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C37" s="1" t="s">
-        <v>341</v>
+        <v>351</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C38" s="1" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C39" s="1" t="s">
-        <v>343</v>
+        <v>353</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C40" s="1" t="s">
-        <v>344</v>
+        <v>354</v>
       </c>
     </row>
   </sheetData>
@@ -5210,176 +5261,176 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="5" width="33.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="5" width="43.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="33.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="43.93"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6" t="s">
-        <v>345</v>
+      <c r="A1" s="5" t="s">
+        <v>355</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>346</v>
+        <v>356</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
-        <v>347</v>
+      <c r="A2" s="6" t="s">
+        <v>357</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>348</v>
+        <v>358</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7" t="s">
-        <v>349</v>
+      <c r="A3" s="6" t="s">
+        <v>359</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>350</v>
+        <v>360</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="s">
-        <v>351</v>
+      <c r="A4" s="6" t="s">
+        <v>361</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>350</v>
+        <v>360</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="s">
-        <v>352</v>
+      <c r="A5" s="6" t="s">
+        <v>362</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>350</v>
+        <v>360</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7" t="s">
-        <v>353</v>
+      <c r="A6" s="6" t="s">
+        <v>363</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>354</v>
+        <v>364</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="7" t="s">
-        <v>355</v>
+      <c r="A7" s="6" t="s">
+        <v>365</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>354</v>
+        <v>364</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7" t="s">
-        <v>356</v>
+      <c r="A8" s="6" t="s">
+        <v>366</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>357</v>
+        <v>367</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7" t="s">
-        <v>358</v>
+      <c r="A9" s="6" t="s">
+        <v>368</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>357</v>
+        <v>367</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="7" t="s">
-        <v>359</v>
+      <c r="A10" s="6" t="s">
+        <v>369</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>357</v>
+        <v>367</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="7" t="s">
-        <v>360</v>
+      <c r="A11" s="6" t="s">
+        <v>370</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>361</v>
+        <v>371</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="7" t="s">
-        <v>362</v>
+      <c r="A12" s="6" t="s">
+        <v>372</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>361</v>
+        <v>371</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="7" t="n">
+      <c r="A13" s="6" t="n">
         <v>620050</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>361</v>
+        <v>371</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="7" t="n">
+      <c r="A14" s="6" t="n">
         <v>7708591995</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>361</v>
+        <v>371</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="7" t="s">
-        <v>363</v>
+      <c r="A15" s="6" t="s">
+        <v>373</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>361</v>
+        <v>371</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="7" t="s">
-        <v>364</v>
+      <c r="A16" s="6" t="s">
+        <v>374</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>365</v>
+        <v>375</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="7" t="s">
-        <v>366</v>
+      <c r="A17" s="6" t="s">
+        <v>376</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>367</v>
+        <v>377</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="7" t="s">
-        <v>368</v>
+      <c r="A18" s="6" t="s">
+        <v>378</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>369</v>
+        <v>379</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="7" t="s">
-        <v>370</v>
+      <c r="A19" s="6" t="s">
+        <v>380</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>371</v>
+        <v>381</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="7" t="s">
-        <v>372</v>
+      <c r="A20" s="6" t="s">
+        <v>382</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>373</v>
+        <v>383</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="7" t="s">
-        <v>374</v>
+      <c r="A21" s="6" t="s">
+        <v>384</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>375</v>
+        <v>385</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: added new columns in file
</commit_message>
<xml_diff>
--- a/unzipping_table.xlsx
+++ b/unzipping_table.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="labels_before_table" sheetId="1" state="visible" r:id="rId3"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="430">
   <si>
     <t xml:space="preserve">seller</t>
   </si>
@@ -621,6 +621,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">CONSIGNEEONSTATION/ПОЛУЧАТЕЛЬПОСТАНЦИИ/</t>
+  </si>
+  <si>
     <t xml:space="preserve">THEBUYER/ПОКУПАТЕЛЬ</t>
   </si>
   <si>
@@ -667,6 +670,9 @@
     <t xml:space="preserve">ПРОДАВЕЦ/THESELLER</t>
   </si>
   <si>
+    <t xml:space="preserve">CONSIGNEE/ПОЛУЧАТЕЛЬ</t>
+  </si>
+  <si>
     <t xml:space="preserve">THEBUYER/ПОКУПАТЕЛЬTHECONSIGNEEE/ПОЛУЧАТЕЛЬ</t>
   </si>
   <si>
@@ -713,6 +719,25 @@
     </r>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ГРУЗОПОЛУЧАТЕЛЬ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">（收货人）</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">ПОКУПАТЕЛЬ/BUYER</t>
   </si>
   <si>
@@ -1024,6 +1049,9 @@
     <t xml:space="preserve">СТАНЦИЯ</t>
   </si>
   <si>
+    <t xml:space="preserve">SHIPPER/ОТПРАВИТЕЛЬ/</t>
+  </si>
+  <si>
     <t xml:space="preserve">SHIPPER/SELLERОТПРАВИТЕЛЬ/ПРОДАВЕЦ</t>
   </si>
   <si>
@@ -1033,6 +1061,25 @@
     <t xml:space="preserve">STATIONOFDESTINATION</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">СТРАНА,ОТПРАВИТЕЛЬ,ПРОДАВЕЦ,АДРЕС</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">（发货人、地址）</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">ОТПРАВИТЕЛЬ/ПРОДАВЕЦ/SHIPPER/SELLER</t>
   </si>
   <si>
@@ -1056,12 +1103,18 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">CТАНЦИЯНАЗНАЧЕНИЯ</t>
+  </si>
+  <si>
     <t xml:space="preserve">ОТПРАВИТЕЛЬ/ПРОДАВЕЦ</t>
   </si>
   <si>
     <t xml:space="preserve">ПОКУПАТЕЛЬСАДРЕСОМ</t>
   </si>
   <si>
+    <t xml:space="preserve">COUNTRYOFDESTINATION/СТРАНАНАЗНАЧЕНИЯSTATIONOFDESTINATION/СТАНЦИЯНАЗНАЧЕНИЯ</t>
+  </si>
+  <si>
     <t xml:space="preserve">ОТПРАВИТЕЛЬ/ПРОДАВЕЦSHIPPER/SELLER</t>
   </si>
   <si>
@@ -1072,6 +1125,25 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
+      <t xml:space="preserve">DESTSTATIONСТАНЦИЯНАЗНАЧЕНИЯ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">目的站</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t xml:space="preserve">ПОКУПАТЕЛЬ/BUYER/</t>
     </r>
     <r>
@@ -1092,6 +1164,25 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
+      <t xml:space="preserve">СТАНЦИЯОТПРАВИТЕЛЯ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">（发站）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t xml:space="preserve">ОТПРАВИТЕЛЬ/ПРОДАВЕЦ</t>
     </r>
     <r>
@@ -1128,9 +1219,15 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">BUYER/ПОЛУЧАТЕЛЬ</t>
+  </si>
+  <si>
     <t xml:space="preserve">SHIPPER(SELLER)</t>
   </si>
   <si>
+    <t xml:space="preserve">ПРОДАВЕЦ/BUYER</t>
+  </si>
+  <si>
     <t xml:space="preserve">ГРУЗОТПРАВИТЕЛЬ(ПРОДАВЕЦ)</t>
   </si>
   <si>
@@ -1287,6 +1384,70 @@
     <t xml:space="preserve">SHIPPERОТПРАВИТЕЛЬ/SELLERПРОДАВЕЦ</t>
   </si>
   <si>
+    <t xml:space="preserve">SUPPLIER/ОТПРАВИТЕЛЬ</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">SHIPPER/SELLERОТПРАВИТЕЛЬ/ПРОДАВЕЦ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">发货人</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">卖家</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ОТПРАВИТЕЛЬ/SHIPPER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">（发货人）</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">SHIPPER/SELLER/SUPPLIERОТПРАВИТЕЛЬ/ПРОДАВЕЦ/ПОСТАВЩИК</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELLERПРОДАВЕЦSHIPPERОТПРАВИТЕЛЬ</t>
+  </si>
+  <si>
     <t xml:space="preserve">model</t>
   </si>
   <si>
@@ -2105,6 +2266,25 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
+      <t xml:space="preserve">NO.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">货物编码序号</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t xml:space="preserve">HSCODE/</t>
     </r>
     <r>
@@ -2874,6 +3054,44 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
+      <t xml:space="preserve">NETWEIGHTKG/НЕТТОКГ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">净重</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GROSSWEIGHTKGБРУТТОКГ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">毛重</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t xml:space="preserve">PRICEPERPCS/ЦЕНАЗАШТ,CNY</t>
     </r>
     <r>
@@ -2986,6 +3204,62 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
+      <t xml:space="preserve">NETWEIGHTKG/ВЕСНЕТТОКГ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">净重</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">/KG</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GROSSWEIGHTKG/ВЕСБРУТТОКГ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">毛重</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">/KG</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t xml:space="preserve">ЦЕНАЗАПАРУ/</t>
     </r>
     <r>
@@ -3136,6 +3410,12 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">N.W.(KG)/ОБЩИЙВЕСНЕТТО(КГ)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G.W.(KG)/ОБЩИЙВЕСБРУТТО(КГ)</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="14"/>
@@ -3289,6 +3569,63 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
+      <t xml:space="preserve">NO.OFPACKAGES/КОЛ-ВОМЕСТ,КОРОБОВ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">大包装件数</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">PRICEPERPCSЦЕНАЗАШТ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">单价</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">AMOUNTСУММА</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">总金额</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t xml:space="preserve">HSCODE/КОДТНВЭДТС</t>
     </r>
     <r>
@@ -3305,12 +3642,144 @@
     <t xml:space="preserve">PRODUCTDESCRIPTION/ОПИСАНИЕТОВАРА.</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">QTYPCS/КОЛ-ВОШТ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">小包装件数</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">TYPEOFPACKAGE/ВИДУПАКОВКИ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">包装类型</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">PRICEPERPCS,CNY/ЦЕНАЗАШТ,ЮАНЬ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">单价</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">元</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">AMOUNT,CNY/ОБЩАЯСТОИМОСТЬ,ЮАНЬ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">金额</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">元</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">CUSTOMSCOMMODITYCODE</t>
   </si>
   <si>
     <t xml:space="preserve">DESCRIPTION/ОПИСАНИЕ</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">QTYPCS/КОЛ-ВОШТ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">数量</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">KINDOFPACKAGE/ВИДУПАКОВКИ</t>
+  </si>
+  <si>
     <t xml:space="preserve">CUSTOMSCOD/КОДТНВЭД</t>
   </si>
   <si>
@@ -3321,6 +3790,28 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
+      <t xml:space="preserve">ОПИСАНИЕГРУЗА</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">俄、英文货物描述</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">QUANTITY/КОЛИЧЕСТВО</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t xml:space="preserve">HSCODE/</t>
     </r>
     <r>
@@ -3337,6 +3828,42 @@
     <r>
       <rPr>
         <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ОПИСАНИЕТОВАРОВ/DESCRIPTIONOFGOODS-РУС.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">品名</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">俄语</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
         <charset val="1"/>
@@ -3354,6 +3881,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">NAMEANDDESCRIPTIONOFGOODS/НАИМЕНОВАНИЕИОПИСАНИЕТОВАРА</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="14"/>
@@ -3381,6 +3911,110 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
+      <t xml:space="preserve">ОПИСАНИЕТОВАРОВ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">（</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ИСПОЛЬЗОВАНИЕПРОДУКТА</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">）</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">/DESCRIPTIONOFGOODS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">（</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">USAGEOFPRODUCT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">）品名描述（用途）（中</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">英</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">俄）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t xml:space="preserve">HSCODE/КОДТНВЭДТСЕАЭС/</t>
     </r>
     <r>
@@ -3595,6 +4229,118 @@
   </si>
   <si>
     <t xml:space="preserve">HSCODE/ТНВЭДТС</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GNGCODE/КОДГНГ</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">HSCODEКОДТНВЭДТС</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">货物编码</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">КОДТНВЭДТС/HSCODE</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">HSCODE/КОДТНВЭДТС</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">海关编码</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">TARIFFCODE/КОДТНВЭД</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H.S.CODE/КОДТОВАРА</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">HSCODE/КОДТНВЭДТС</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">国外清关</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">HSCODE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">（非国内报关</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">HS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">）</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">С</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">station</t>
@@ -3697,7 +4443,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -3744,6 +4490,11 @@
       <name val="Noto Sans CJK SC"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="Noto Sans CJK SC"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -3952,12 +4703,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+      <selection pane="bottomLeft" activeCell="E29" activeCellId="0" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4239,223 +4990,281 @@
       <c r="B15" s="1" t="s">
         <v>79</v>
       </c>
+      <c r="C15" s="1" t="s">
+        <v>80</v>
+      </c>
       <c r="D15" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>121</v>
+      </c>
       <c r="B25" s="1" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>125</v>
+      </c>
       <c r="B26" s="1" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>122</v>
+        <v>127</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="1" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>124</v>
+        <v>130</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="1" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="E28" s="1" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="1" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>126</v>
+        <v>134</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="1" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="1" t="s">
-        <v>129</v>
+        <v>138</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="1" t="s">
-        <v>130</v>
+        <v>140</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="1" t="s">
-        <v>131</v>
+        <v>142</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="1" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="1" t="s">
-        <v>133</v>
+        <v>144</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="1" t="s">
-        <v>134</v>
+        <v>145</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="1" t="s">
-        <v>135</v>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="1" t="s">
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -4474,12 +5283,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K40"/>
+  <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="K22" activeCellId="0" sqref="K22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="E29" activeCellId="0" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4500,739 +5309,837 @@
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>136</v>
+        <v>152</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>137</v>
+        <v>153</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>138</v>
+        <v>154</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>139</v>
+        <v>155</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>140</v>
+        <v>156</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>141</v>
+        <v>157</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>142</v>
+        <v>158</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>143</v>
+        <v>159</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>144</v>
+        <v>160</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>145</v>
+        <v>161</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>146</v>
+        <v>162</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>147</v>
+        <v>163</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>148</v>
+        <v>164</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>149</v>
+        <v>165</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>150</v>
+        <v>166</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>151</v>
+        <v>167</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>152</v>
+        <v>168</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>153</v>
+        <v>169</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>154</v>
+        <v>170</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>155</v>
+        <v>171</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>156</v>
+        <v>172</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>157</v>
+        <v>173</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>158</v>
+        <v>174</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>159</v>
+        <v>175</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>160</v>
+        <v>176</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>161</v>
+        <v>177</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>162</v>
+        <v>178</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>163</v>
+        <v>179</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>164</v>
+        <v>180</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>165</v>
+        <v>181</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>166</v>
+        <v>182</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>167</v>
+        <v>183</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>168</v>
+        <v>184</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
-        <v>169</v>
+        <v>185</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>170</v>
+        <v>186</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>171</v>
+        <v>187</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>172</v>
+        <v>188</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>173</v>
+        <v>189</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>174</v>
+        <v>190</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>175</v>
+        <v>191</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>176</v>
+        <v>192</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>177</v>
+        <v>193</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>178</v>
+        <v>194</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="1" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>181</v>
+        <v>197</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>182</v>
+        <v>198</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>183</v>
+        <v>199</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>184</v>
+        <v>200</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>185</v>
+        <v>201</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>186</v>
+        <v>202</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="1" t="s">
-        <v>189</v>
+        <v>205</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>190</v>
+        <v>206</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>191</v>
+        <v>207</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>192</v>
+        <v>208</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>193</v>
+        <v>209</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>194</v>
+        <v>210</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>195</v>
+        <v>211</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>196</v>
+        <v>212</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>197</v>
+        <v>213</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>198</v>
+        <v>214</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="1" t="s">
-        <v>199</v>
+        <v>215</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>200</v>
+        <v>216</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>201</v>
+        <v>217</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>202</v>
+        <v>218</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>203</v>
+        <v>219</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>204</v>
+        <v>220</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>205</v>
+        <v>221</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>206</v>
+        <v>222</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>207</v>
+        <v>223</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>208</v>
+        <v>224</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1" t="s">
-        <v>209</v>
+        <v>225</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>210</v>
+        <v>226</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>211</v>
+        <v>227</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>212</v>
+        <v>228</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>213</v>
+        <v>229</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>214</v>
+        <v>230</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>215</v>
+        <v>231</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>216</v>
+        <v>232</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>217</v>
+        <v>233</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>218</v>
+        <v>234</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="1" t="s">
-        <v>219</v>
+        <v>235</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>220</v>
+        <v>236</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>221</v>
+        <v>237</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>222</v>
+        <v>238</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>223</v>
+        <v>239</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>224</v>
+        <v>240</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>225</v>
+        <v>241</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>226</v>
+        <v>242</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>227</v>
+        <v>243</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>228</v>
+        <v>244</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="1" t="s">
-        <v>229</v>
+        <v>245</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>230</v>
+        <v>246</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>231</v>
+        <v>247</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>232</v>
+        <v>248</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>233</v>
+        <v>249</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>234</v>
+        <v>250</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>235</v>
+        <v>251</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>236</v>
+        <v>252</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>237</v>
+        <v>253</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>238</v>
+        <v>254</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="1" t="s">
-        <v>239</v>
+        <v>255</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>240</v>
+        <v>256</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>241</v>
+        <v>257</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>242</v>
+        <v>258</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>243</v>
+        <v>259</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>244</v>
+        <v>260</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>245</v>
+        <v>261</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>246</v>
+        <v>262</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>247</v>
+        <v>263</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>248</v>
+        <v>264</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="1" t="s">
+        <v>265</v>
+      </c>
       <c r="C12" s="1" t="s">
-        <v>249</v>
+        <v>266</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>250</v>
+        <v>267</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>251</v>
+        <v>268</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>252</v>
+        <v>269</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>253</v>
+        <v>270</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>254</v>
+        <v>271</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>255</v>
+        <v>272</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>256</v>
+        <v>273</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>257</v>
+        <v>274</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="1" t="s">
-        <v>258</v>
+        <v>275</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>259</v>
+        <v>276</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>260</v>
+        <v>277</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>261</v>
+        <v>278</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>262</v>
+        <v>279</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>263</v>
+        <v>280</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>264</v>
+        <v>281</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>265</v>
+        <v>282</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>266</v>
+        <v>283</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="1" t="s">
-        <v>267</v>
+        <v>284</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>268</v>
+        <v>285</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>269</v>
+        <v>286</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>270</v>
+        <v>287</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>271</v>
+        <v>288</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>272</v>
+        <v>289</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>273</v>
+        <v>290</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>274</v>
+        <v>291</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>275</v>
+        <v>292</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="1" t="s">
-        <v>276</v>
+        <v>293</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>277</v>
+        <v>294</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>278</v>
+        <v>295</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>279</v>
+        <v>296</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>280</v>
+        <v>297</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>281</v>
+        <v>298</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>282</v>
+        <v>299</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>283</v>
+        <v>300</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>284</v>
+        <v>301</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="1" t="s">
-        <v>285</v>
+        <v>302</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>286</v>
+        <v>303</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>287</v>
+        <v>304</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>288</v>
+        <v>305</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>289</v>
+        <v>306</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>290</v>
+        <v>307</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>291</v>
+        <v>308</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>292</v>
+        <v>309</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C17" s="1" t="s">
-        <v>293</v>
+        <v>310</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>294</v>
+        <v>311</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>295</v>
+        <v>312</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>296</v>
+        <v>313</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>297</v>
+        <v>314</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>298</v>
+        <v>315</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>299</v>
+        <v>316</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>300</v>
+        <v>317</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C18" s="1" t="s">
-        <v>301</v>
+        <v>318</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>302</v>
+        <v>319</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>303</v>
+        <v>320</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>304</v>
+        <v>321</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>305</v>
+        <v>322</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>306</v>
+        <v>323</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>307</v>
+        <v>324</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>308</v>
+        <v>325</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C19" s="1" t="s">
-        <v>309</v>
+        <v>326</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>310</v>
+        <v>327</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>311</v>
+        <v>328</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>312</v>
+        <v>329</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>331</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>313</v>
+        <v>332</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>314</v>
+        <v>333</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C20" s="1" t="s">
-        <v>315</v>
+        <v>334</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>316</v>
+        <v>335</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>317</v>
+        <v>336</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>318</v>
+        <v>337</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>339</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>319</v>
+        <v>340</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>320</v>
+        <v>341</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="1" t="s">
-        <v>321</v>
+        <v>342</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>322</v>
+        <v>343</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>323</v>
+        <v>344</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>324</v>
+        <v>345</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>347</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>325</v>
+        <v>348</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>326</v>
+        <v>349</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C22" s="3" t="s">
-        <v>327</v>
+        <v>350</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>328</v>
+        <v>351</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>329</v>
+        <v>352</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>330</v>
+        <v>353</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>331</v>
+        <v>354</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>332</v>
+        <v>355</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C23" s="1" t="s">
-        <v>333</v>
+        <v>356</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>334</v>
+        <v>357</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>335</v>
+        <v>358</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>361</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C24" s="1" t="s">
-        <v>336</v>
+        <v>362</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>363</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C25" s="1" t="s">
-        <v>338</v>
+        <v>368</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>369</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C26" s="1" t="s">
-        <v>340</v>
+        <v>372</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>374</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C27" s="1" t="s">
-        <v>341</v>
+        <v>375</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>376</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C28" s="3" t="s">
-        <v>342</v>
+        <v>377</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>378</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C29" s="1" t="s">
-        <v>343</v>
+        <v>379</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>380</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C30" s="1" t="s">
-        <v>344</v>
+        <v>381</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C31" s="1" t="s">
-        <v>345</v>
+        <v>382</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C32" s="1" t="s">
-        <v>346</v>
+        <v>383</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C33" s="1" t="s">
-        <v>347</v>
+        <v>384</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="1" t="s">
-        <v>348</v>
+        <v>385</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C35" s="1" t="s">
-        <v>349</v>
+        <v>386</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C36" s="1" t="s">
-        <v>350</v>
+        <v>387</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C37" s="1" t="s">
-        <v>351</v>
+        <v>388</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C38" s="1" t="s">
-        <v>352</v>
+        <v>389</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C39" s="1" t="s">
-        <v>353</v>
+        <v>390</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C40" s="1" t="s">
-        <v>354</v>
+        <v>391</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C41" s="1" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C42" s="1" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C43" s="1" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C44" s="1" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C45" s="1" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C46" s="1" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C47" s="1" t="s">
+        <v>398</v>
       </c>
     </row>
   </sheetData>
@@ -5267,98 +6174,98 @@
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>355</v>
+        <v>399</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>356</v>
+        <v>400</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>357</v>
+        <v>401</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>358</v>
+        <v>402</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>359</v>
+        <v>403</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>360</v>
+        <v>404</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>361</v>
+        <v>405</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>360</v>
+        <v>404</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>362</v>
+        <v>406</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>360</v>
+        <v>404</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>363</v>
+        <v>407</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>364</v>
+        <v>408</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>365</v>
+        <v>409</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>364</v>
+        <v>408</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>366</v>
+        <v>410</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>367</v>
+        <v>411</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>368</v>
+        <v>412</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>367</v>
+        <v>411</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
-        <v>369</v>
+        <v>413</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>367</v>
+        <v>411</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
-        <v>370</v>
+        <v>414</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>371</v>
+        <v>415</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
-        <v>372</v>
+        <v>416</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>371</v>
+        <v>415</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5366,7 +6273,7 @@
         <v>620050</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>371</v>
+        <v>415</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5374,63 +6281,63 @@
         <v>7708591995</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>371</v>
+        <v>415</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
-        <v>373</v>
+        <v>417</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>371</v>
+        <v>415</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
-        <v>374</v>
+        <v>418</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>375</v>
+        <v>419</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
-        <v>376</v>
+        <v>420</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>377</v>
+        <v>421</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
-        <v>378</v>
+        <v>422</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>379</v>
+        <v>423</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="s">
-        <v>380</v>
+        <v>424</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>381</v>
+        <v>425</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="6" t="s">
-        <v>382</v>
+        <v>426</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>383</v>
+        <v>427</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="6" t="s">
-        <v>384</v>
+        <v>428</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>385</v>
+        <v>429</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add: added handling of delivery terms
</commit_message>
<xml_diff>
--- a/unzipping_table.xlsx
+++ b/unzipping_table.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="labels_before_table" sheetId="1" state="visible" r:id="rId3"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="481">
   <si>
     <t xml:space="preserve">seller</t>
   </si>
@@ -42,6 +42,9 @@
     <t xml:space="preserve">container_number</t>
   </si>
   <si>
+    <t xml:space="preserve">delivery_terms</t>
+  </si>
+  <si>
     <t xml:space="preserve">SHIPPER/ГРУЗООТПРАВИТЕЛЬ</t>
   </si>
   <si>
@@ -60,6 +63,9 @@
     <t xml:space="preserve">CONTAINER/КОНТЕЙНЕР</t>
   </si>
   <si>
+    <t xml:space="preserve">DELIVERYTERMS/УСЛОВИЯПОСТАВКИ</t>
+  </si>
+  <si>
     <t xml:space="preserve">SHIPPER/ОТПРАВИТЕЛЬ</t>
   </si>
   <si>
@@ -112,6 +118,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">TERMSOFDELIVERY/УСЛОВИЯПОСТАВКИ</t>
+  </si>
+  <si>
     <t xml:space="preserve">SHIPPER/ОТПРАВИТЕЛЬ(SAMEASSMGS'SHIPPER)</t>
   </si>
   <si>
@@ -137,6 +146,26 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
+      <t xml:space="preserve">TERMSOFDELIVERYУСЛОВИЯПОСТАВКИ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">运输条款</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t xml:space="preserve">SHIPPER/ОТПРАВИТЕЛЬ/</t>
     </r>
     <r>
@@ -172,6 +201,26 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
+      <t xml:space="preserve">УСЛОВИЯПОСТАВКИ/TERMSOFDELIVERY/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">交付條款</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t xml:space="preserve">SHIPPER</t>
     </r>
     <r>
@@ -234,6 +283,9 @@
     <t xml:space="preserve">CONTAINER/КОНТЕЙНЕРNO.</t>
   </si>
   <si>
+    <t xml:space="preserve">TERMSOFDELIVERY/УСЛОВИЯПОСТАВКИ/</t>
+  </si>
+  <si>
     <t xml:space="preserve">THECONSIGNOR/ОТПРАВИТЕЛЬ</t>
   </si>
   <si>
@@ -303,6 +355,9 @@
     <t xml:space="preserve">CONTAINER/КОНТЕЙНЕР/</t>
   </si>
   <si>
+    <t xml:space="preserve">TERMSOFDELIVERY</t>
+  </si>
+  <si>
     <t xml:space="preserve">THESENDER/ОТПРАВИТЕЛЬ</t>
   </si>
   <si>
@@ -372,6 +427,35 @@
     </r>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">TERMSOFDELIVERY/УСЛОВИЯ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">交货方式</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">CONTAINER/КОНТЕЙНЕР</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">THESHIPPER/ОТПРАВИТЕЛЬ</t>
   </si>
   <si>
@@ -387,6 +471,26 @@
     <t xml:space="preserve">STATIONOFDESTINATIONСТАНЦИЯНАЗНАЧЕНИЯ</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">TERMSOFDELIVERY/УСЛОВИЯПОСТАВКИ/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">交货条款</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">ГРУЗОТПРАВИТЕЛЬ/SHIPPER</t>
   </si>
   <si>
@@ -419,6 +523,26 @@
     <t xml:space="preserve">СТАНЦИЯНАЗНАЧЕНИЯ</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">УСЛОВИЯПОСТАВКИ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">供货条件</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">ОТПРАВИТЕЛЬ</t>
   </si>
   <si>
@@ -434,6 +558,9 @@
     <t xml:space="preserve">СТАНЦИЯНАЗНАЧЕНИЯ(DESTINATIONSTATION)</t>
   </si>
   <si>
+    <t xml:space="preserve">УСЛОВИЯПОСТАВКИ(TERMSOFDELIVERY)</t>
+  </si>
+  <si>
     <t xml:space="preserve">ОТПРАВИТЕЛЬ/SHIPPER</t>
   </si>
   <si>
@@ -483,6 +610,9 @@
     <t xml:space="preserve">СТАНЦИЯНАЗНАЧЕНИЯ/DESTINATIONSTATION</t>
   </si>
   <si>
+    <t xml:space="preserve">УСЛОВИЯПОСТАВКИ/TERMSOFDELIVERY</t>
+  </si>
+  <si>
     <t xml:space="preserve">ОТПРАВИТЕЛЬ/THESENDER</t>
   </si>
   <si>
@@ -549,6 +679,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">УСЛОВИЯПОСТАВКИ</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="14"/>
@@ -581,6 +714,9 @@
     <t xml:space="preserve">СТРАНАНАЗНАЧЕНИЯСТАНЦИЯНАЗНАЧЕНИЯ</t>
   </si>
   <si>
+    <t xml:space="preserve">DELIVERYTERMS</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="14"/>
@@ -647,6 +783,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">TERMSOFPAYMENT/УСЛОВИЯПОСТАВКИ</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="14"/>
@@ -696,6 +835,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">TERMSOFDELIVERY/</t>
+  </si>
+  <si>
     <t xml:space="preserve">SHIPFROM/ОТПРАВИТЕЛЬ</t>
   </si>
   <si>
@@ -769,6 +911,26 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
+      <t xml:space="preserve">TERMSOFDELIVERY/УСЛОВИЯПОСТАВКИ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">贸易方式</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t xml:space="preserve">ОТПРАВИТЕЛЬ/SHIPPER</t>
     </r>
     <r>
@@ -799,6 +961,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">收货人及地址</t>
     </r>
@@ -816,6 +979,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">添加运单第四栏公司和地址</t>
     </r>
@@ -853,6 +1017,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">TERMSOFDELIVERYУСЛОВИЯПОСТАВКИ</t>
+  </si>
+  <si>
     <t xml:space="preserve">ПРОДАВЕЦ/ОТПРАВИТЕЛЬСАДРЕСОМ</t>
   </si>
   <si>
@@ -902,6 +1069,26 @@
     <r>
       <rPr>
         <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">运输条款</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">/УСЛОВИЯПОСТАВКИ</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="1"/>
@@ -928,6 +1115,26 @@
     <t xml:space="preserve">目的站</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">TERMSOFDELIVERY/УСЛОВИЯПОСТАВКИ/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">贸易条款</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">CONSIGNOR/ГРУЗООТПРАВИТЕЛЬ</t>
   </si>
   <si>
@@ -957,6 +1164,9 @@
     <t xml:space="preserve">RECEIVINGSTATION/СТАНЦИЯНАЗНАЧЕНИЯ</t>
   </si>
   <si>
+    <t xml:space="preserve">TRADETERMS/УСЛОВИЯПОСТАВКИ</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="14"/>
@@ -1020,6 +1230,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">TERMSOFDELIVERY/УСЛОВИЯПОСТАВКИCHENGDU,CHINA</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="14"/>
@@ -1095,6 +1308,9 @@
     <t xml:space="preserve">СТАНЦИЯ</t>
   </si>
   <si>
+    <t xml:space="preserve">TERMSOFDELIVERY/УСЛОВИЯ</t>
+  </si>
+  <si>
     <t xml:space="preserve">SHIPPER/ОТПРАВИТЕЛЬ/</t>
   </si>
   <si>
@@ -1107,6 +1323,9 @@
     <t xml:space="preserve">STATIONOFDESTINATION</t>
   </si>
   <si>
+    <t xml:space="preserve">TERMS/УСЛОВИЯПОСТАВКИ</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="14"/>
@@ -1179,6 +1398,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">发货人及地址</t>
     </r>
@@ -1196,6 +1416,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">添加运单第一栏公司和地址</t>
     </r>
@@ -1247,6 +1468,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">发货人及地址（添加运单第一栏公司和地址）</t>
     </r>
@@ -1286,6 +1508,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">目的站</t>
     </r>
@@ -1340,25 +1563,6 @@
     <t xml:space="preserve">BUYER/ПОЛУЧАТЕЛЬ</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">СТАНЦИЯПРИБЫТИЯ/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">到达站</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">SHIPPER(SELLER)</t>
   </si>
   <si>
@@ -1385,6 +1589,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">收货人及地址</t>
     </r>
@@ -1402,6 +1607,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">添加运单第四栏公司和地址</t>
     </r>
@@ -1545,6 +1751,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">买方</t>
     </r>
@@ -1562,6 +1769,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">收货人</t>
     </r>
@@ -1689,6 +1897,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">卖方及地址</t>
     </r>
@@ -1708,6 +1917,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">卖方及地址</t>
     </r>
@@ -1727,6 +1937,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">卖方</t>
     </r>
@@ -1744,6 +1955,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">发货人</t>
     </r>
@@ -2698,6 +2910,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">序号</t>
     </r>
@@ -3816,6 +4029,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">净重</t>
     </r>
@@ -3833,6 +4047,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">，</t>
     </r>
@@ -3852,6 +4067,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">毛重</t>
     </r>
@@ -3869,6 +4085,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">，</t>
     </r>
@@ -4201,6 +4418,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">单价</t>
     </r>
@@ -4220,6 +4438,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">总价</t>
     </r>
@@ -4265,6 +4484,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">件数</t>
     </r>
@@ -4282,6 +4502,357 @@
     <r>
       <rPr>
         <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">编码</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">HSCODE/КОДТНВЭДТС</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ОПИСАНИЕТОВАРОВ/DESCRIPTIONOFGOODS-РУС.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">品名</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">俄语</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">个数</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">QTYPCS/КОЛ-ВОШТ</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">HSCODE/КОДТНВЭДТС</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">欧洲段税号</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">NAMEANDDESCRIPTIONOFGOODS/НАИМЕНОВАНИЕИОПИСАНИЕТОВАРА</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">HSCODE/КОДТНВЭДТСЕАЭС/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">海关编码</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ОПИСАНИЕТОВАРОВ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">（</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ИСПОЛЬЗОВАНИЕПРОДУКТА</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">）</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">/DESCRIPTIONOFGOODS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">（</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">USAGEOFPRODUCT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">）品名描述（用途）（中</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">英</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">俄）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">HSCODE/КОДТНВЭДТС</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">商编</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">英俄文品名</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">DESCRIPTIONOFGOODSОПИСАНИЕТОВАРОВ</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">КОДТНВЭДРФ/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">海关编码</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">HSCODE/КОДТНВЭДТС/HS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">编码</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">HSCODE/КОДТНВЭДТС10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">位</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">HSCODE/КОДТНВЭДТС</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">商编（按运单商编添加）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="1"/>
@@ -4295,67 +4866,76 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
+      <t xml:space="preserve">海关编码（目的国</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">HS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">编码）</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">HSCODE/КОДТОВАРА</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">HSCODE/КОДТНВЭДТС</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t xml:space="preserve">海关编码</t>
     </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">ОПИСАНИЕТОВАРОВ/DESCRIPTIONOFGOODS-РУС.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">品名</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">俄语</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">个数</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">QTYPCS/КОЛ-ВОШТ</t>
-    </r>
-  </si>
-  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">/CU</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">HS</t>
+    </r>
     <r>
       <rPr>
         <sz val="14"/>
@@ -4365,6 +4945,40 @@
       </rPr>
       <t xml:space="preserve">编码</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">HSCODE/КОДТНВЭДТС/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HSCODE/ТНВЭДТС</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GNGCODE/КОДГНГ</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">HSCODEКОДТНВЭДТС</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">货物编码</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">КОДТНВЭДТС/HSCODE</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="14"/>
@@ -4374,9 +4988,21 @@
       </rPr>
       <t xml:space="preserve">HSCODE/КОДТНВЭДТС</t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">NAMEANDDESCRIPTIONOFGOODS/НАИМЕНОВАНИЕИОПИСАНИЕТОВАРА</t>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">海关编码</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">TARIFFCODE/КОДТНВЭД</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H.S.CODE/КОДТОВАРА</t>
   </si>
   <si>
     <r>
@@ -4395,36 +5021,34 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">欧洲段税号</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">ОПИСАНИЕТОВАРОВ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">（</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">ИСПОЛЬЗОВАНИЕПРОДУКТА</t>
+      <t xml:space="preserve">国外清关</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">HSCODE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">（非国内报关</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">HS</t>
     </r>
     <r>
       <rPr>
@@ -4442,109 +5066,57 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">/DESCRIPTIONOFGOODS</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">（</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">USAGEOFPRODUCT</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">）品名描述（用途）（中</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">+</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">英</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">+</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">俄）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">HSCODE/КОДТНВЭДТСЕАЭС/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">海关编码</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">英俄文品名</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">DESCRIPTIONOFGOODSОПИСАНИЕТОВАРОВ</t>
+      <t xml:space="preserve">С</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">HSCODE/HSКОДДЛЯТАМОЖ.ОФОРМЛЕНИЯВКНР</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">HSCODE/КОДТНВЭДТС/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">商编</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">按运单商编添加</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
     </r>
   </si>
   <si>
@@ -4564,67 +5136,25 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">商编</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">КОДТНВЭДРФ/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">海关编码</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">HSCODE/КОДТНВЭДТС/HS</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">编码</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">HSCODE/КОДТНВЭДТС10</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">位</t>
+      <t xml:space="preserve">（海关编码</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">位）</t>
     </r>
   </si>
   <si>
@@ -4644,329 +5174,6 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">商编（按运单商编添加）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">HSCODE/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">海关编码（目的国</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">HS</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">编码）</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">HSCODE/КОДТОВАРА</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">HSCODE/КОДТНВЭДТС</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">海关编码</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">/CU</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">HS</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">编码</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">HSCODE/КОДТНВЭДТС/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HSCODE/ТНВЭДТС</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GNGCODE/КОДГНГ</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">HSCODEКОДТНВЭДТС</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">货物编码</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">КОДТНВЭДТС/HSCODE</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">HSCODE/КОДТНВЭДТС</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">海关编码</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">TARIFFCODE/КОДТНВЭД</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H.S.CODE/КОДТОВАРА</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">HSCODE/КОДТНВЭДТС</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">国外清关</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">HSCODE</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">（非国内报关</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">HS</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">）</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">С</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">HSCODE/HSКОДДЛЯТАМОЖ.ОФОРМЛЕНИЯВКНР</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">HSCODE/КОДТНВЭДТС/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">商编</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">按运单商编添加</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">HSCODE/КОДТНВЭДТС</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">（海关编码</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">10</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">位）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">HSCODE/КОДТНВЭДТС</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-      </rPr>
       <t xml:space="preserve">商品编码</t>
     </r>
   </si>
@@ -4976,6 +5183,7 @@
         <sz val="14"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">海关编码</t>
     </r>
@@ -5090,7 +5298,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -5137,11 +5345,6 @@
       <name val="Noto Sans CJK SC"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <name val="Noto Sans CJK SC"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -5197,7 +5400,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -5211,10 +5414,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5354,12 +5553,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F48"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E32" activeCellId="0" sqref="E32"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="G25" activeCellId="0" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5369,7 +5568,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="20.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="28.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="32.41"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="6" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="42.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="30.05"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="8" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5391,591 +5592,666 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>19</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>54</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>52</v>
+        <v>60</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>57</v>
+        <v>66</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>62</v>
+        <v>72</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>67</v>
+        <v>78</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>72</v>
+        <v>84</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>77</v>
+        <v>90</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>81</v>
+        <v>95</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>82</v>
+        <v>96</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>83</v>
+        <v>98</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>84</v>
+        <v>99</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>87</v>
+        <v>102</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>89</v>
+        <v>105</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>90</v>
+        <v>106</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>91</v>
+        <v>107</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>92</v>
+        <v>108</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>95</v>
+        <v>112</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>96</v>
+        <v>113</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>97</v>
+        <v>114</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>98</v>
+        <v>116</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>99</v>
+        <v>117</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>100</v>
+        <v>118</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>101</v>
+        <v>119</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>102</v>
+        <v>121</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>103</v>
+        <v>122</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>104</v>
+        <v>123</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>105</v>
+        <v>124</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>106</v>
+        <v>126</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>107</v>
+        <v>127</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>108</v>
+        <v>128</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>109</v>
+        <v>129</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>110</v>
+        <v>131</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>111</v>
+        <v>132</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>112</v>
+        <v>133</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>113</v>
+        <v>134</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>114</v>
+        <v>136</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>115</v>
+        <v>137</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>116</v>
+        <v>138</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>117</v>
+        <v>139</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>118</v>
+        <v>140</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>119</v>
+        <v>141</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>120</v>
+        <v>142</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>121</v>
+        <v>143</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>122</v>
+        <v>145</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>123</v>
+        <v>146</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>124</v>
+        <v>147</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>125</v>
+        <v>148</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>126</v>
+        <v>150</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>127</v>
+        <v>151</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>128</v>
+        <v>152</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>129</v>
+        <v>153</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>130</v>
+        <v>154</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>131</v>
+        <v>155</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>132</v>
+        <v>156</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>133</v>
+        <v>157</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>134</v>
+        <v>158</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>135</v>
+        <v>159</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>136</v>
+        <v>160</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>137</v>
+        <v>161</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>138</v>
+        <v>162</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>139</v>
+        <v>163</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="1" t="s">
-        <v>140</v>
+        <v>164</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>141</v>
+        <v>165</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>142</v>
+        <v>166</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="1" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>144</v>
+        <v>168</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>145</v>
+        <v>114</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="1" t="s">
-        <v>146</v>
+        <v>169</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>147</v>
+        <v>170</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>148</v>
+        <v>171</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="1" t="s">
-        <v>149</v>
+        <v>172</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>150</v>
+        <v>173</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="1" t="s">
-        <v>151</v>
+        <v>174</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>152</v>
+        <v>175</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="1" t="s">
-        <v>153</v>
+        <v>176</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>154</v>
+        <v>177</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="1" t="s">
-        <v>155</v>
+        <v>178</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="1" t="s">
-        <v>156</v>
+        <v>179</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="1" t="s">
-        <v>157</v>
+        <v>180</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="1" t="s">
-        <v>158</v>
+        <v>181</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="1" t="s">
-        <v>159</v>
+        <v>182</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="1" t="s">
-        <v>160</v>
+        <v>183</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="1" t="s">
-        <v>161</v>
+        <v>184</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="1" t="s">
-        <v>162</v>
+        <v>185</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="1" t="s">
-        <v>163</v>
+        <v>186</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="1" t="s">
-        <v>164</v>
+        <v>187</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="1" t="s">
-        <v>165</v>
+        <v>188</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="1" t="s">
-        <v>166</v>
+        <v>189</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="1" t="s">
-        <v>167</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>
@@ -5994,12 +6270,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K52"/>
+  <dimension ref="A1:K51"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="K25" activeCellId="0" sqref="K25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="C27" activeCellId="0" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6020,886 +6296,881 @@
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>168</v>
+        <v>191</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>169</v>
+        <v>192</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>170</v>
+        <v>193</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>171</v>
+        <v>194</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>172</v>
+        <v>195</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>173</v>
+        <v>196</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>174</v>
+        <v>197</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>175</v>
+        <v>198</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>176</v>
+        <v>199</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>177</v>
+        <v>200</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>178</v>
+        <v>201</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>179</v>
+        <v>202</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>180</v>
+        <v>203</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>181</v>
+        <v>204</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>182</v>
+        <v>205</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>183</v>
+        <v>206</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>184</v>
+        <v>207</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>185</v>
+        <v>208</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>186</v>
+        <v>209</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>187</v>
+        <v>210</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>189</v>
+        <v>212</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>190</v>
+        <v>213</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>191</v>
+        <v>214</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>192</v>
+        <v>215</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>193</v>
+        <v>216</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>194</v>
+        <v>217</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>195</v>
+        <v>218</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>196</v>
+        <v>219</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>197</v>
+        <v>220</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>198</v>
+        <v>221</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>199</v>
+        <v>222</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>200</v>
+        <v>223</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
-        <v>201</v>
+        <v>224</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>202</v>
+        <v>225</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>203</v>
+        <v>226</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>204</v>
+        <v>227</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>205</v>
+        <v>228</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>206</v>
+        <v>229</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>207</v>
+        <v>230</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>208</v>
+        <v>231</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>209</v>
+        <v>232</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>210</v>
+        <v>233</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="1" t="s">
-        <v>211</v>
+        <v>234</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>212</v>
+        <v>235</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>213</v>
+        <v>236</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>214</v>
+        <v>237</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>215</v>
+        <v>238</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>216</v>
+        <v>239</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>217</v>
+        <v>240</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>218</v>
+        <v>241</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>219</v>
+        <v>242</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>220</v>
+        <v>243</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="1" t="s">
-        <v>221</v>
+        <v>244</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>222</v>
+        <v>245</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>223</v>
+        <v>246</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>224</v>
+        <v>247</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>225</v>
+        <v>248</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>226</v>
+        <v>249</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>227</v>
+        <v>250</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>228</v>
+        <v>251</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>229</v>
+        <v>252</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>230</v>
+        <v>253</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="1" t="s">
-        <v>231</v>
+        <v>254</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>232</v>
+        <v>255</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>233</v>
+        <v>256</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>234</v>
+        <v>257</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>235</v>
+        <v>258</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>236</v>
+        <v>259</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>237</v>
+        <v>260</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>238</v>
+        <v>261</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>239</v>
+        <v>262</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>240</v>
+        <v>263</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1" t="s">
-        <v>241</v>
+        <v>264</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>242</v>
+        <v>265</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>243</v>
+        <v>266</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>244</v>
+        <v>267</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>245</v>
+        <v>268</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>246</v>
+        <v>269</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>247</v>
+        <v>270</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>248</v>
+        <v>271</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>249</v>
+        <v>272</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>250</v>
+        <v>273</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="1" t="s">
-        <v>251</v>
+        <v>274</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>252</v>
+        <v>275</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>253</v>
+        <v>276</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>254</v>
+        <v>277</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>255</v>
+        <v>278</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>256</v>
+        <v>279</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>257</v>
+        <v>280</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>258</v>
+        <v>281</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>259</v>
+        <v>282</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>260</v>
+        <v>283</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="1" t="s">
-        <v>261</v>
+        <v>284</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>262</v>
+        <v>285</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>263</v>
+        <v>286</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>264</v>
+        <v>287</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>265</v>
+        <v>288</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>266</v>
+        <v>289</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>267</v>
+        <v>290</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>268</v>
+        <v>291</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>269</v>
+        <v>292</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>270</v>
+        <v>293</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="1" t="s">
-        <v>271</v>
+        <v>294</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>272</v>
+        <v>295</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>273</v>
+        <v>296</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>274</v>
+        <v>297</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>275</v>
+        <v>298</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>276</v>
+        <v>299</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>277</v>
+        <v>300</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>278</v>
+        <v>301</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>279</v>
+        <v>302</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>280</v>
+        <v>303</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="1" t="s">
-        <v>281</v>
+        <v>304</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>282</v>
+        <v>305</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>283</v>
+        <v>306</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>284</v>
+        <v>307</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>285</v>
+        <v>308</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>286</v>
+        <v>309</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>287</v>
+        <v>310</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>288</v>
+        <v>311</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>289</v>
+        <v>312</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>290</v>
+        <v>313</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="4" t="s">
-        <v>291</v>
+      <c r="B13" s="3" t="s">
+        <v>314</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>292</v>
+        <v>315</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>293</v>
+        <v>316</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>294</v>
+        <v>317</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>295</v>
+        <v>318</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>296</v>
+        <v>319</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>297</v>
+        <v>320</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>298</v>
+        <v>321</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>299</v>
+        <v>322</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>300</v>
+        <v>323</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="1" t="s">
-        <v>301</v>
+        <v>324</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>302</v>
+        <v>325</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>303</v>
+        <v>326</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>304</v>
+        <v>327</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>305</v>
+        <v>328</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>306</v>
+        <v>329</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>307</v>
+        <v>330</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>308</v>
+        <v>331</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>309</v>
+        <v>332</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="1" t="s">
-        <v>310</v>
+        <v>333</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>311</v>
+        <v>334</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>312</v>
+        <v>335</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>313</v>
+        <v>336</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>314</v>
+        <v>337</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>315</v>
+        <v>338</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>316</v>
+        <v>339</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>317</v>
+        <v>340</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>318</v>
+        <v>341</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="1" t="s">
-        <v>319</v>
+        <v>342</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>320</v>
+        <v>343</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>321</v>
+        <v>344</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>322</v>
+        <v>345</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>323</v>
+        <v>346</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>324</v>
+        <v>347</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>325</v>
+        <v>348</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>326</v>
+        <v>349</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C17" s="1" t="s">
-        <v>327</v>
+        <v>350</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>328</v>
+        <v>351</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>329</v>
+        <v>352</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>330</v>
+        <v>353</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>331</v>
+        <v>354</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>332</v>
+        <v>355</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>333</v>
+        <v>356</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>334</v>
+        <v>357</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C18" s="1" t="s">
-        <v>335</v>
+        <v>358</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>336</v>
+        <v>359</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>337</v>
+        <v>360</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>338</v>
+        <v>361</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>339</v>
+        <v>362</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>340</v>
+        <v>363</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>341</v>
+        <v>364</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>342</v>
+        <v>365</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C19" s="1" t="s">
-        <v>343</v>
+        <v>366</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>344</v>
+        <v>367</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>345</v>
+        <v>368</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>346</v>
+        <v>369</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>347</v>
+        <v>370</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>348</v>
+        <v>371</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>349</v>
+        <v>372</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>350</v>
+        <v>373</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C20" s="1" t="s">
-        <v>351</v>
+        <v>374</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>352</v>
+        <v>375</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>353</v>
+        <v>376</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>354</v>
+        <v>377</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>355</v>
+        <v>378</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>356</v>
+        <v>379</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>357</v>
+        <v>380</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>358</v>
+        <v>381</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="1" t="s">
-        <v>359</v>
+        <v>382</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>360</v>
+        <v>383</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>361</v>
+        <v>384</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>362</v>
+        <v>385</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>363</v>
+        <v>386</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>364</v>
+        <v>387</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>365</v>
+        <v>388</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>366</v>
+        <v>389</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C22" s="3" t="s">
-        <v>367</v>
+        <v>390</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>368</v>
+        <v>391</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>369</v>
+        <v>392</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>370</v>
-      </c>
-      <c r="H22" s="4" t="s">
-        <v>371</v>
-      </c>
-      <c r="I22" s="4" t="s">
-        <v>372</v>
+        <v>393</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>394</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>395</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>373</v>
+        <v>396</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>374</v>
+        <v>397</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C23" s="1" t="s">
-        <v>375</v>
+        <v>398</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>376</v>
+        <v>399</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>377</v>
+        <v>400</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>378</v>
+        <v>401</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>379</v>
+        <v>402</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>380</v>
+        <v>403</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C24" s="1" t="s">
-        <v>381</v>
+        <v>404</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>382</v>
+        <v>405</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>383</v>
+        <v>406</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>384</v>
+        <v>407</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>385</v>
+        <v>408</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>386</v>
+        <v>409</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C25" s="1" t="s">
-        <v>387</v>
+        <v>410</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>388</v>
+        <v>411</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>389</v>
+        <v>412</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="J25" s="4" t="s">
-        <v>391</v>
-      </c>
-      <c r="K25" s="4" t="s">
-        <v>392</v>
+        <v>413</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>414</v>
+      </c>
+      <c r="K25" s="3" t="s">
+        <v>415</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C26" s="1" t="s">
-        <v>393</v>
+        <v>416</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>394</v>
+        <v>417</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>395</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>396</v>
+        <v>418</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>419</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C27" s="1" t="s">
-        <v>397</v>
+      <c r="C27" s="3" t="s">
+        <v>420</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>398</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>399</v>
+        <v>421</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C28" s="3" t="s">
-        <v>400</v>
+      <c r="C28" s="1" t="s">
+        <v>423</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>401</v>
+        <v>424</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C29" s="1" t="s">
-        <v>402</v>
+        <v>425</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>403</v>
+        <v>426</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C30" s="1" t="s">
-        <v>404</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>405</v>
+        <v>427</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C31" s="1" t="s">
-        <v>406</v>
+        <v>429</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C32" s="1" t="s">
-        <v>407</v>
+        <v>430</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C33" s="1" t="s">
-        <v>408</v>
+        <v>431</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="1" t="s">
-        <v>409</v>
+        <v>432</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C35" s="1" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C36" s="1" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C37" s="1" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C38" s="1" t="s">
-        <v>413</v>
+        <v>436</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C39" s="1" t="s">
-        <v>414</v>
+        <v>437</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C40" s="1" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C41" s="1" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C42" s="1" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C43" s="1" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C44" s="1" t="s">
-        <v>419</v>
+        <v>442</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C45" s="1" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C46" s="1" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C47" s="1" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C48" s="1" t="s">
-        <v>423</v>
+        <v>446</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C49" s="1" t="s">
-        <v>424</v>
+        <v>447</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C50" s="1" t="s">
-        <v>425</v>
+        <v>448</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C51" s="1" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C52" s="4" t="s">
-        <v>427</v>
+      <c r="C51" s="3" t="s">
+        <v>449</v>
       </c>
     </row>
   </sheetData>
@@ -6928,176 +7199,176 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="5" width="33.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="5" width="43.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="33.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="43.93"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6" t="s">
-        <v>428</v>
+      <c r="A1" s="5" t="s">
+        <v>450</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>429</v>
+        <v>451</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
-        <v>430</v>
+      <c r="A2" s="6" t="s">
+        <v>452</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>431</v>
+        <v>453</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7" t="s">
-        <v>432</v>
+      <c r="A3" s="6" t="s">
+        <v>454</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>433</v>
+        <v>455</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="s">
-        <v>434</v>
+      <c r="A4" s="6" t="s">
+        <v>456</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>433</v>
+        <v>455</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="s">
-        <v>435</v>
+      <c r="A5" s="6" t="s">
+        <v>457</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>433</v>
+        <v>455</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7" t="s">
-        <v>436</v>
+      <c r="A6" s="6" t="s">
+        <v>458</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>437</v>
+        <v>459</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="7" t="s">
-        <v>438</v>
+      <c r="A7" s="6" t="s">
+        <v>460</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>437</v>
+        <v>459</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7" t="s">
-        <v>439</v>
+      <c r="A8" s="6" t="s">
+        <v>461</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>440</v>
+        <v>462</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7" t="s">
-        <v>441</v>
+      <c r="A9" s="6" t="s">
+        <v>463</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>440</v>
+        <v>462</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="7" t="s">
-        <v>442</v>
+      <c r="A10" s="6" t="s">
+        <v>464</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>440</v>
+        <v>462</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="7" t="s">
-        <v>443</v>
+      <c r="A11" s="6" t="s">
+        <v>465</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>444</v>
+        <v>466</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="7" t="s">
-        <v>445</v>
+      <c r="A12" s="6" t="s">
+        <v>467</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>444</v>
+        <v>466</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="7" t="n">
+      <c r="A13" s="6" t="n">
         <v>620050</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>444</v>
+        <v>466</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="7" t="n">
+      <c r="A14" s="6" t="n">
         <v>7708591995</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>444</v>
+        <v>466</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="7" t="s">
-        <v>446</v>
+      <c r="A15" s="6" t="s">
+        <v>468</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>444</v>
+        <v>466</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="7" t="s">
-        <v>447</v>
+      <c r="A16" s="6" t="s">
+        <v>469</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>448</v>
+        <v>470</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="7" t="s">
-        <v>449</v>
+      <c r="A17" s="6" t="s">
+        <v>471</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>450</v>
+        <v>472</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="7" t="s">
-        <v>451</v>
+      <c r="A18" s="6" t="s">
+        <v>473</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>452</v>
+        <v>474</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="7" t="s">
-        <v>453</v>
+      <c r="A19" s="6" t="s">
+        <v>475</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>454</v>
+        <v>476</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="7" t="s">
-        <v>455</v>
+      <c r="A20" s="6" t="s">
+        <v>477</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>456</v>
+        <v>478</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="7" t="s">
-        <v>457</v>
+      <c r="A21" s="6" t="s">
+        <v>479</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>458</v>
+        <v>480</v>
       </c>
     </row>
   </sheetData>

</xml_diff>